<commit_message>
chinh sua yeu cau thay doi
</commit_message>
<xml_diff>
--- a/Busy schedule - Fr teachers 20160220.xlsx
+++ b/Busy schedule - Fr teachers 20160220.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" tabRatio="964"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" tabRatio="964" firstSheet="5" activeTab="29"/>
   </bookViews>
   <sheets>
     <sheet name="Alec" sheetId="16" r:id="rId1"/>
@@ -36,7 +36,11 @@
     <sheet name="Todd" sheetId="2" r:id="rId27"/>
     <sheet name="Tom" sheetId="1" r:id="rId28"/>
     <sheet name="Tony W" sheetId="30" r:id="rId29"/>
+    <sheet name="Hoang" sheetId="42" r:id="rId30"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId31"/>
+  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Alec!$A$6:$J$27</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -51,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="58">
   <si>
     <t>*) Notes:</t>
   </si>
@@ -222,6 +226,9 @@
   </si>
   <si>
     <t>Week from 22-02 to 28-02</t>
+  </si>
+  <si>
+    <t>Hoang</t>
   </si>
 </sst>
 </file>
@@ -880,7 +887,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="238">
+  <cellXfs count="240">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1465,6 +1472,42 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1474,60 +1517,42 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1543,23 +1568,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1612,6 +1625,74 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Bao"/>
+      <sheetName val="Hanh"/>
+      <sheetName val="Hao"/>
+      <sheetName val="Hao tutor"/>
+      <sheetName val="Hoang"/>
+      <sheetName val="Huy"/>
+      <sheetName val="Kieu My"/>
+      <sheetName val="K.Khanh"/>
+      <sheetName val="Lan"/>
+      <sheetName val="Ng. Uyen"/>
+      <sheetName val="Nhan"/>
+      <sheetName val="Nguyen"/>
+      <sheetName val="Thanh My"/>
+      <sheetName val="T.Thao"/>
+      <sheetName val="T.Truc"/>
+      <sheetName val="Kha Thi"/>
+      <sheetName val="Thoan"/>
+      <sheetName val="Trang"/>
+      <sheetName val="Truc"/>
+      <sheetName val="Tuan"/>
+      <sheetName val="Tuan tutor"/>
+      <sheetName val="Tung tutor"/>
+      <sheetName val="Uyen"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>Week from 22-02 to 28-02</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="B6">
+            <v>42422</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1869,7 +1950,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1880,7 +1961,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
@@ -1977,7 +2058,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" s="119" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="232" t="s">
+      <c r="A7" s="206" t="s">
         <v>40</v>
       </c>
       <c r="B7" s="27"/>
@@ -1990,7 +2071,7 @@
       <c r="I7" s="118"/>
     </row>
     <row r="8" spans="1:9" s="119" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="233"/>
+      <c r="A8" s="207"/>
       <c r="B8" s="22"/>
       <c r="C8" s="22"/>
       <c r="D8" s="124"/>
@@ -2001,7 +2082,7 @@
       <c r="I8" s="118"/>
     </row>
     <row r="9" spans="1:9" s="119" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="233"/>
+      <c r="A9" s="207"/>
       <c r="B9" s="30"/>
       <c r="C9" s="22"/>
       <c r="D9" s="125"/>
@@ -2012,7 +2093,7 @@
       <c r="I9" s="118"/>
     </row>
     <row r="10" spans="1:9" s="119" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="234"/>
+      <c r="A10" s="208"/>
       <c r="B10" s="53"/>
       <c r="C10" s="23"/>
       <c r="D10" s="126"/>
@@ -2023,7 +2104,7 @@
       <c r="I10" s="118"/>
     </row>
     <row r="11" spans="1:9" s="119" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="213" t="s">
+      <c r="A11" s="215" t="s">
         <v>31</v>
       </c>
       <c r="B11" s="12"/>
@@ -2036,7 +2117,7 @@
       <c r="I11" s="118"/>
     </row>
     <row r="12" spans="1:9" s="119" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="214"/>
+      <c r="A12" s="216"/>
       <c r="B12" s="22"/>
       <c r="C12" s="22"/>
       <c r="D12" s="29"/>
@@ -2047,7 +2128,7 @@
       <c r="I12" s="118"/>
     </row>
     <row r="13" spans="1:9" s="119" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="214"/>
+      <c r="A13" s="216"/>
       <c r="B13" s="22"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
@@ -2058,7 +2139,7 @@
       <c r="I13" s="118"/>
     </row>
     <row r="14" spans="1:9" s="119" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="215"/>
+      <c r="A14" s="217"/>
       <c r="B14" s="49"/>
       <c r="C14" s="49"/>
       <c r="D14" s="49"/>
@@ -2069,7 +2150,7 @@
       <c r="I14" s="118"/>
     </row>
     <row r="15" spans="1:9" s="119" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="213" t="s">
+      <c r="A15" s="215" t="s">
         <v>32</v>
       </c>
       <c r="B15" s="12"/>
@@ -2082,7 +2163,7 @@
       <c r="I15" s="118"/>
     </row>
     <row r="16" spans="1:9" s="119" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="214"/>
+      <c r="A16" s="216"/>
       <c r="B16" s="22"/>
       <c r="C16" s="22"/>
       <c r="D16" s="29"/>
@@ -2093,7 +2174,7 @@
       <c r="I16" s="118"/>
     </row>
     <row r="17" spans="1:10" s="119" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="214"/>
+      <c r="A17" s="216"/>
       <c r="B17" s="22"/>
       <c r="C17" s="22"/>
       <c r="D17" s="22"/>
@@ -2104,7 +2185,7 @@
       <c r="I17" s="118"/>
     </row>
     <row r="18" spans="1:10" s="119" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="215"/>
+      <c r="A18" s="217"/>
       <c r="B18" s="49"/>
       <c r="C18" s="49"/>
       <c r="D18" s="49"/>
@@ -2115,7 +2196,7 @@
       <c r="I18" s="118"/>
     </row>
     <row r="19" spans="1:10" s="119" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="209" t="s">
+      <c r="A19" s="212" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="12"/>
@@ -2128,7 +2209,7 @@
       <c r="I19" s="118"/>
     </row>
     <row r="20" spans="1:10" s="119" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="210"/>
+      <c r="A20" s="213"/>
       <c r="B20" s="22"/>
       <c r="C20" s="22"/>
       <c r="D20" s="22"/>
@@ -2139,7 +2220,7 @@
       <c r="I20" s="118"/>
     </row>
     <row r="21" spans="1:10" s="119" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="210"/>
+      <c r="A21" s="213"/>
       <c r="B21" s="87"/>
       <c r="C21" s="22"/>
       <c r="D21" s="22"/>
@@ -2150,7 +2231,7 @@
       <c r="I21" s="118"/>
     </row>
     <row r="22" spans="1:10" s="119" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="211"/>
+      <c r="A22" s="214"/>
       <c r="B22" s="22"/>
       <c r="C22" s="23"/>
       <c r="D22" s="23"/>
@@ -2161,7 +2242,7 @@
       <c r="I22" s="118"/>
     </row>
     <row r="23" spans="1:10" s="119" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="235" t="s">
+      <c r="A23" s="209" t="s">
         <v>1</v>
       </c>
       <c r="B23" s="12"/>
@@ -2174,7 +2255,7 @@
       <c r="I23" s="118"/>
     </row>
     <row r="24" spans="1:10" s="119" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="236"/>
+      <c r="A24" s="210"/>
       <c r="B24" s="22"/>
       <c r="C24" s="22"/>
       <c r="D24" s="34"/>
@@ -2185,7 +2266,7 @@
       <c r="I24" s="118"/>
     </row>
     <row r="25" spans="1:10" s="119" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="236"/>
+      <c r="A25" s="210"/>
       <c r="B25" s="22"/>
       <c r="C25" s="22"/>
       <c r="D25" s="34"/>
@@ -2196,7 +2277,7 @@
       <c r="I25" s="118"/>
     </row>
     <row r="26" spans="1:10" s="119" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="237"/>
+      <c r="A26" s="211"/>
       <c r="B26" s="54"/>
       <c r="C26" s="54"/>
       <c r="D26" s="35"/>
@@ -2370,7 +2451,7 @@
       <c r="J6" s="14"/>
     </row>
     <row r="7" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="207" t="s">
+      <c r="A7" s="219" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="22"/>
@@ -2383,7 +2464,7 @@
       <c r="I7" s="14"/>
     </row>
     <row r="8" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="207"/>
+      <c r="A8" s="219"/>
       <c r="B8" s="22"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
@@ -2394,7 +2475,7 @@
       <c r="I8" s="14"/>
     </row>
     <row r="9" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="207"/>
+      <c r="A9" s="219"/>
       <c r="B9" s="22"/>
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
@@ -2405,7 +2486,7 @@
       <c r="I9" s="14"/>
     </row>
     <row r="10" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="208"/>
+      <c r="A10" s="220"/>
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>
       <c r="D10" s="23"/>
@@ -2416,7 +2497,7 @@
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="209" t="s">
+      <c r="A11" s="212" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="84"/>
@@ -2429,7 +2510,7 @@
       <c r="I11" s="14"/>
     </row>
     <row r="12" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="224"/>
+      <c r="A12" s="229"/>
       <c r="B12" s="85"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
@@ -2440,7 +2521,7 @@
       <c r="I12" s="14"/>
     </row>
     <row r="13" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="224"/>
+      <c r="A13" s="229"/>
       <c r="B13" s="85"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
@@ -2451,7 +2532,7 @@
       <c r="I13" s="14"/>
     </row>
     <row r="14" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="226"/>
+      <c r="A14" s="231"/>
       <c r="B14" s="86"/>
       <c r="C14" s="49"/>
       <c r="D14" s="49"/>
@@ -2462,7 +2543,7 @@
       <c r="I14" s="14"/>
     </row>
     <row r="15" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="223" t="s">
+      <c r="A15" s="228" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="12"/>
@@ -2475,7 +2556,7 @@
       <c r="I15" s="14"/>
     </row>
     <row r="16" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="224"/>
+      <c r="A16" s="229"/>
       <c r="B16" s="22"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
@@ -2486,7 +2567,7 @@
       <c r="I16" s="14"/>
     </row>
     <row r="17" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="224"/>
+      <c r="A17" s="229"/>
       <c r="B17" s="22"/>
       <c r="C17" s="22"/>
       <c r="D17" s="22"/>
@@ -2497,7 +2578,7 @@
       <c r="I17" s="14"/>
     </row>
     <row r="18" spans="1:9" s="40" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="225"/>
+      <c r="A18" s="230"/>
       <c r="B18" s="58"/>
       <c r="C18" s="50"/>
       <c r="D18" s="54"/>
@@ -2637,7 +2718,7 @@
       <c r="J6" s="14"/>
     </row>
     <row r="7" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="207" t="s">
+      <c r="A7" s="219" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="22"/>
@@ -2650,7 +2731,7 @@
       <c r="I7" s="14"/>
     </row>
     <row r="8" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="207"/>
+      <c r="A8" s="219"/>
       <c r="B8" s="22"/>
       <c r="C8" s="34"/>
       <c r="D8" s="22"/>
@@ -2661,7 +2742,7 @@
       <c r="I8" s="14"/>
     </row>
     <row r="9" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="207"/>
+      <c r="A9" s="219"/>
       <c r="B9" s="22"/>
       <c r="C9" s="34"/>
       <c r="D9" s="22"/>
@@ -2672,7 +2753,7 @@
       <c r="I9" s="14"/>
     </row>
     <row r="10" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="208"/>
+      <c r="A10" s="220"/>
       <c r="B10" s="23"/>
       <c r="C10" s="60"/>
       <c r="D10" s="23"/>
@@ -2683,7 +2764,7 @@
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="1:10" s="40" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="207" t="s">
+      <c r="A11" s="219" t="s">
         <v>31</v>
       </c>
       <c r="B11" s="22"/>
@@ -2696,7 +2777,7 @@
       <c r="I11" s="14"/>
     </row>
     <row r="12" spans="1:10" s="40" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="207"/>
+      <c r="A12" s="219"/>
       <c r="B12" s="22"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
@@ -2707,7 +2788,7 @@
       <c r="I12" s="14"/>
     </row>
     <row r="13" spans="1:10" s="40" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="207"/>
+      <c r="A13" s="219"/>
       <c r="B13" s="22"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
@@ -2718,7 +2799,7 @@
       <c r="I13" s="14"/>
     </row>
     <row r="14" spans="1:10" s="40" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="208"/>
+      <c r="A14" s="220"/>
       <c r="B14" s="49"/>
       <c r="C14" s="53"/>
       <c r="D14" s="49"/>
@@ -2729,7 +2810,7 @@
       <c r="I14" s="14"/>
     </row>
     <row r="15" spans="1:10" s="40" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="207" t="s">
+      <c r="A15" s="219" t="s">
         <v>32</v>
       </c>
       <c r="B15" s="22"/>
@@ -2742,7 +2823,7 @@
       <c r="I15" s="14"/>
     </row>
     <row r="16" spans="1:10" s="40" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="207"/>
+      <c r="A16" s="219"/>
       <c r="B16" s="22"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
@@ -2753,7 +2834,7 @@
       <c r="I16" s="14"/>
     </row>
     <row r="17" spans="1:9" s="40" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="207"/>
+      <c r="A17" s="219"/>
       <c r="B17" s="22"/>
       <c r="C17" s="22"/>
       <c r="D17" s="22"/>
@@ -2764,7 +2845,7 @@
       <c r="I17" s="14"/>
     </row>
     <row r="18" spans="1:9" s="40" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="208"/>
+      <c r="A18" s="220"/>
       <c r="B18" s="49"/>
       <c r="C18" s="53"/>
       <c r="D18" s="49"/>
@@ -2775,7 +2856,7 @@
       <c r="I18" s="14"/>
     </row>
     <row r="19" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="209" t="s">
+      <c r="A19" s="212" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="12"/>
@@ -2788,7 +2869,7 @@
       <c r="I19" s="14"/>
     </row>
     <row r="20" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="224"/>
+      <c r="A20" s="229"/>
       <c r="B20" s="22"/>
       <c r="C20" s="22"/>
       <c r="D20" s="34"/>
@@ -2799,7 +2880,7 @@
       <c r="I20" s="14"/>
     </row>
     <row r="21" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="224"/>
+      <c r="A21" s="229"/>
       <c r="B21" s="87"/>
       <c r="C21" s="22"/>
       <c r="D21" s="34"/>
@@ -2810,7 +2891,7 @@
       <c r="I21" s="14"/>
     </row>
     <row r="22" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="226"/>
+      <c r="A22" s="231"/>
       <c r="B22" s="49"/>
       <c r="C22" s="53"/>
       <c r="D22" s="66"/>
@@ -2821,7 +2902,7 @@
       <c r="I22" s="14"/>
     </row>
     <row r="23" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="223" t="s">
+      <c r="A23" s="228" t="s">
         <v>1</v>
       </c>
       <c r="B23" s="12"/>
@@ -2834,7 +2915,7 @@
       <c r="I23" s="14"/>
     </row>
     <row r="24" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="224"/>
+      <c r="A24" s="229"/>
       <c r="B24" s="22"/>
       <c r="C24" s="22"/>
       <c r="D24" s="22"/>
@@ -2845,7 +2926,7 @@
       <c r="I24" s="14"/>
     </row>
     <row r="25" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="224"/>
+      <c r="A25" s="229"/>
       <c r="B25" s="22"/>
       <c r="C25" s="22"/>
       <c r="D25" s="22"/>
@@ -2856,7 +2937,7 @@
       <c r="I25" s="14"/>
     </row>
     <row r="26" spans="1:9" s="40" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="225"/>
+      <c r="A26" s="230"/>
       <c r="B26" s="58"/>
       <c r="C26" s="54"/>
       <c r="D26" s="54"/>
@@ -2998,7 +3079,7 @@
       <c r="J6" s="14"/>
     </row>
     <row r="7" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="213" t="s">
+      <c r="A7" s="215" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="22"/>
@@ -3011,7 +3092,7 @@
       <c r="I7" s="14"/>
     </row>
     <row r="8" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="214"/>
+      <c r="A8" s="216"/>
       <c r="B8" s="22"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
@@ -3022,7 +3103,7 @@
       <c r="I8" s="14"/>
     </row>
     <row r="9" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="214"/>
+      <c r="A9" s="216"/>
       <c r="B9" s="22"/>
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
@@ -3033,7 +3114,7 @@
       <c r="I9" s="14"/>
     </row>
     <row r="10" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="215"/>
+      <c r="A10" s="217"/>
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>
       <c r="D10" s="23"/>
@@ -3044,7 +3125,7 @@
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="207" t="s">
+      <c r="A11" s="219" t="s">
         <v>31</v>
       </c>
       <c r="B11" s="22"/>
@@ -3057,7 +3138,7 @@
       <c r="I11" s="14"/>
     </row>
     <row r="12" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="207"/>
+      <c r="A12" s="219"/>
       <c r="B12" s="22"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
@@ -3068,7 +3149,7 @@
       <c r="I12" s="14"/>
     </row>
     <row r="13" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="207"/>
+      <c r="A13" s="219"/>
       <c r="B13" s="22"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
@@ -3079,7 +3160,7 @@
       <c r="I13" s="14"/>
     </row>
     <row r="14" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="208"/>
+      <c r="A14" s="220"/>
       <c r="B14" s="53"/>
       <c r="C14" s="53"/>
       <c r="D14" s="49"/>
@@ -3090,7 +3171,7 @@
       <c r="I14" s="14"/>
     </row>
     <row r="15" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="213" t="s">
+      <c r="A15" s="215" t="s">
         <v>32</v>
       </c>
       <c r="B15" s="22"/>
@@ -3103,7 +3184,7 @@
       <c r="I15" s="14"/>
     </row>
     <row r="16" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="214"/>
+      <c r="A16" s="216"/>
       <c r="B16" s="22"/>
       <c r="C16" s="22"/>
       <c r="D16" s="31"/>
@@ -3114,7 +3195,7 @@
       <c r="I16" s="14"/>
     </row>
     <row r="17" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="214"/>
+      <c r="A17" s="216"/>
       <c r="B17" s="22"/>
       <c r="C17" s="22"/>
       <c r="D17" s="31"/>
@@ -3125,7 +3206,7 @@
       <c r="I17" s="14"/>
     </row>
     <row r="18" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="214"/>
+      <c r="A18" s="216"/>
       <c r="B18" s="30"/>
       <c r="C18" s="30"/>
       <c r="D18" s="31"/>
@@ -3136,7 +3217,7 @@
       <c r="I18" s="14"/>
     </row>
     <row r="19" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="213" t="s">
+      <c r="A19" s="215" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="115"/>
@@ -3149,7 +3230,7 @@
       <c r="I19" s="14"/>
     </row>
     <row r="20" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="214"/>
+      <c r="A20" s="216"/>
       <c r="B20" s="78"/>
       <c r="C20" s="78"/>
       <c r="D20" s="78"/>
@@ -3160,7 +3241,7 @@
       <c r="I20" s="14"/>
     </row>
     <row r="21" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="214"/>
+      <c r="A21" s="216"/>
       <c r="B21" s="78"/>
       <c r="C21" s="78"/>
       <c r="D21" s="78"/>
@@ -3171,7 +3252,7 @@
       <c r="I21" s="14"/>
     </row>
     <row r="22" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="215"/>
+      <c r="A22" s="217"/>
       <c r="B22" s="30"/>
       <c r="C22" s="30"/>
       <c r="D22" s="31"/>
@@ -3182,7 +3263,7 @@
       <c r="I22" s="14"/>
     </row>
     <row r="23" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="209" t="s">
+      <c r="A23" s="212" t="s">
         <v>1</v>
       </c>
       <c r="B23" s="12"/>
@@ -3195,7 +3276,7 @@
       <c r="I23" s="14"/>
     </row>
     <row r="24" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="224"/>
+      <c r="A24" s="229"/>
       <c r="B24" s="22"/>
       <c r="C24" s="22"/>
       <c r="D24" s="22"/>
@@ -3206,7 +3287,7 @@
       <c r="I24" s="14"/>
     </row>
     <row r="25" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="224"/>
+      <c r="A25" s="229"/>
       <c r="B25" s="22"/>
       <c r="C25" s="22"/>
       <c r="D25" s="22"/>
@@ -3217,7 +3298,7 @@
       <c r="I25" s="14"/>
     </row>
     <row r="26" spans="1:9" s="40" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="225"/>
+      <c r="A26" s="230"/>
       <c r="B26" s="50"/>
       <c r="C26" s="58"/>
       <c r="D26" s="54"/>
@@ -3360,7 +3441,7 @@
       <c r="J6" s="14"/>
     </row>
     <row r="7" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="213" t="s">
+      <c r="A7" s="215" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="22"/>
@@ -3373,7 +3454,7 @@
       <c r="I7" s="14"/>
     </row>
     <row r="8" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="214"/>
+      <c r="A8" s="216"/>
       <c r="B8" s="22"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
@@ -3384,7 +3465,7 @@
       <c r="I8" s="14"/>
     </row>
     <row r="9" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="214"/>
+      <c r="A9" s="216"/>
       <c r="B9" s="22"/>
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
@@ -3395,7 +3476,7 @@
       <c r="I9" s="14"/>
     </row>
     <row r="10" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="215"/>
+      <c r="A10" s="217"/>
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>
       <c r="D10" s="23"/>
@@ -3406,7 +3487,7 @@
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="1:10" s="40" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="207" t="s">
+      <c r="A11" s="219" t="s">
         <v>31</v>
       </c>
       <c r="B11" s="22"/>
@@ -3419,7 +3500,7 @@
       <c r="I11" s="14"/>
     </row>
     <row r="12" spans="1:10" s="40" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="207"/>
+      <c r="A12" s="219"/>
       <c r="B12" s="22"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
@@ -3430,7 +3511,7 @@
       <c r="I12" s="14"/>
     </row>
     <row r="13" spans="1:10" s="40" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="207"/>
+      <c r="A13" s="219"/>
       <c r="B13" s="22"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
@@ -3441,7 +3522,7 @@
       <c r="I13" s="14"/>
     </row>
     <row r="14" spans="1:10" s="40" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="208"/>
+      <c r="A14" s="220"/>
       <c r="B14" s="53"/>
       <c r="C14" s="53"/>
       <c r="D14" s="49"/>
@@ -3452,7 +3533,7 @@
       <c r="I14" s="14"/>
     </row>
     <row r="15" spans="1:10" s="40" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="213" t="s">
+      <c r="A15" s="215" t="s">
         <v>32</v>
       </c>
       <c r="B15" s="22"/>
@@ -3465,7 +3546,7 @@
       <c r="I15" s="14"/>
     </row>
     <row r="16" spans="1:10" s="40" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="214"/>
+      <c r="A16" s="216"/>
       <c r="B16" s="22"/>
       <c r="C16" s="22"/>
       <c r="D16" s="31"/>
@@ -3476,7 +3557,7 @@
       <c r="I16" s="14"/>
     </row>
     <row r="17" spans="1:9" s="40" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="214"/>
+      <c r="A17" s="216"/>
       <c r="B17" s="22"/>
       <c r="C17" s="22"/>
       <c r="D17" s="31"/>
@@ -3487,7 +3568,7 @@
       <c r="I17" s="14"/>
     </row>
     <row r="18" spans="1:9" s="40" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="214"/>
+      <c r="A18" s="216"/>
       <c r="B18" s="30"/>
       <c r="C18" s="30"/>
       <c r="D18" s="31"/>
@@ -3498,7 +3579,7 @@
       <c r="I18" s="14"/>
     </row>
     <row r="19" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="213" t="s">
+      <c r="A19" s="215" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="115"/>
@@ -3511,7 +3592,7 @@
       <c r="I19" s="14"/>
     </row>
     <row r="20" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="214"/>
+      <c r="A20" s="216"/>
       <c r="B20" s="78"/>
       <c r="C20" s="78"/>
       <c r="D20" s="78"/>
@@ -3522,7 +3603,7 @@
       <c r="I20" s="14"/>
     </row>
     <row r="21" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="214"/>
+      <c r="A21" s="216"/>
       <c r="B21" s="78"/>
       <c r="C21" s="78"/>
       <c r="D21" s="78"/>
@@ -3533,7 +3614,7 @@
       <c r="I21" s="14"/>
     </row>
     <row r="22" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="215"/>
+      <c r="A22" s="217"/>
       <c r="B22" s="30"/>
       <c r="C22" s="30"/>
       <c r="D22" s="31"/>
@@ -3544,7 +3625,7 @@
       <c r="I22" s="14"/>
     </row>
     <row r="23" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="209" t="s">
+      <c r="A23" s="212" t="s">
         <v>1</v>
       </c>
       <c r="B23" s="12"/>
@@ -3557,7 +3638,7 @@
       <c r="I23" s="14"/>
     </row>
     <row r="24" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="224"/>
+      <c r="A24" s="229"/>
       <c r="B24" s="22"/>
       <c r="C24" s="22"/>
       <c r="D24" s="22"/>
@@ -3568,7 +3649,7 @@
       <c r="I24" s="14"/>
     </row>
     <row r="25" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="224"/>
+      <c r="A25" s="229"/>
       <c r="B25" s="22"/>
       <c r="C25" s="22"/>
       <c r="D25" s="22"/>
@@ -3579,7 +3660,7 @@
       <c r="I25" s="14"/>
     </row>
     <row r="26" spans="1:9" s="40" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="225"/>
+      <c r="A26" s="230"/>
       <c r="B26" s="50"/>
       <c r="C26" s="50"/>
       <c r="D26" s="54"/>
@@ -3717,7 +3798,7 @@
       <c r="J6" s="14"/>
     </row>
     <row r="7" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="207" t="s">
+      <c r="A7" s="219" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="22"/>
@@ -3730,7 +3811,7 @@
       <c r="I7" s="14"/>
     </row>
     <row r="8" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="207"/>
+      <c r="A8" s="219"/>
       <c r="B8" s="22"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
@@ -3741,7 +3822,7 @@
       <c r="I8" s="14"/>
     </row>
     <row r="9" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="207"/>
+      <c r="A9" s="219"/>
       <c r="B9" s="22"/>
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
@@ -3752,7 +3833,7 @@
       <c r="I9" s="14"/>
     </row>
     <row r="10" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="208"/>
+      <c r="A10" s="220"/>
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>
       <c r="D10" s="23"/>
@@ -3763,7 +3844,7 @@
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="209" t="s">
+      <c r="A11" s="212" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="27"/>
@@ -3776,7 +3857,7 @@
       <c r="I11" s="14"/>
     </row>
     <row r="12" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="224"/>
+      <c r="A12" s="229"/>
       <c r="B12" s="22"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
@@ -3787,7 +3868,7 @@
       <c r="I12" s="14"/>
     </row>
     <row r="13" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="224"/>
+      <c r="A13" s="229"/>
       <c r="B13" s="22"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
@@ -3798,7 +3879,7 @@
       <c r="I13" s="14"/>
     </row>
     <row r="14" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="226"/>
+      <c r="A14" s="231"/>
       <c r="B14" s="135"/>
       <c r="C14" s="135"/>
       <c r="D14" s="49"/>
@@ -3809,7 +3890,7 @@
       <c r="I14" s="14"/>
     </row>
     <row r="15" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="223" t="s">
+      <c r="A15" s="228" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="12"/>
@@ -3822,7 +3903,7 @@
       <c r="I15" s="14"/>
     </row>
     <row r="16" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="224"/>
+      <c r="A16" s="229"/>
       <c r="B16" s="22"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
@@ -3833,7 +3914,7 @@
       <c r="I16" s="14"/>
     </row>
     <row r="17" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="224"/>
+      <c r="A17" s="229"/>
       <c r="B17" s="22"/>
       <c r="C17" s="22"/>
       <c r="D17" s="22"/>
@@ -3844,7 +3925,7 @@
       <c r="I17" s="14"/>
     </row>
     <row r="18" spans="1:9" s="40" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="225"/>
+      <c r="A18" s="230"/>
       <c r="B18" s="58"/>
       <c r="C18" s="58"/>
       <c r="D18" s="54"/>
@@ -3987,7 +4068,7 @@
       <c r="J6" s="14"/>
     </row>
     <row r="7" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="216" t="s">
+      <c r="A7" s="221" t="s">
         <v>40</v>
       </c>
       <c r="B7" s="22"/>
@@ -4000,7 +4081,7 @@
       <c r="I7" s="14"/>
     </row>
     <row r="8" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="216"/>
+      <c r="A8" s="221"/>
       <c r="B8" s="22"/>
       <c r="C8" s="22"/>
       <c r="D8" s="34"/>
@@ -4011,7 +4092,7 @@
       <c r="I8" s="14"/>
     </row>
     <row r="9" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="216"/>
+      <c r="A9" s="221"/>
       <c r="B9" s="22"/>
       <c r="C9" s="22"/>
       <c r="D9" s="34"/>
@@ -4022,7 +4103,7 @@
       <c r="I9" s="14"/>
     </row>
     <row r="10" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="217"/>
+      <c r="A10" s="222"/>
       <c r="B10" s="53"/>
       <c r="C10" s="23"/>
       <c r="D10" s="47"/>
@@ -4033,7 +4114,7 @@
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="213" t="s">
+      <c r="A11" s="215" t="s">
         <v>31</v>
       </c>
       <c r="B11" s="22"/>
@@ -4046,7 +4127,7 @@
       <c r="I11" s="14"/>
     </row>
     <row r="12" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="214"/>
+      <c r="A12" s="216"/>
       <c r="B12" s="22"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
@@ -4057,7 +4138,7 @@
       <c r="I12" s="14"/>
     </row>
     <row r="13" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="214"/>
+      <c r="A13" s="216"/>
       <c r="B13" s="22"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
@@ -4068,7 +4149,7 @@
       <c r="I13" s="14"/>
     </row>
     <row r="14" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="215"/>
+      <c r="A14" s="217"/>
       <c r="B14" s="49"/>
       <c r="C14" s="49"/>
       <c r="D14" s="49"/>
@@ -4079,7 +4160,7 @@
       <c r="I14" s="14"/>
     </row>
     <row r="15" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="227" t="s">
+      <c r="A15" s="233" t="s">
         <v>32</v>
       </c>
       <c r="B15" s="22"/>
@@ -4092,7 +4173,7 @@
       <c r="I15" s="14"/>
     </row>
     <row r="16" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="224"/>
+      <c r="A16" s="229"/>
       <c r="B16" s="22"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
@@ -4103,7 +4184,7 @@
       <c r="I16" s="14"/>
     </row>
     <row r="17" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="224"/>
+      <c r="A17" s="229"/>
       <c r="B17" s="22"/>
       <c r="C17" s="22"/>
       <c r="D17" s="22"/>
@@ -4114,7 +4195,7 @@
       <c r="I17" s="14"/>
     </row>
     <row r="18" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="226"/>
+      <c r="A18" s="231"/>
       <c r="B18" s="49"/>
       <c r="C18" s="49"/>
       <c r="D18" s="49"/>
@@ -4125,7 +4206,7 @@
       <c r="I18" s="14"/>
     </row>
     <row r="19" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="223" t="s">
+      <c r="A19" s="228" t="s">
         <v>1</v>
       </c>
       <c r="B19" s="12"/>
@@ -4138,7 +4219,7 @@
       <c r="I19" s="14"/>
     </row>
     <row r="20" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="224"/>
+      <c r="A20" s="229"/>
       <c r="B20" s="22"/>
       <c r="C20" s="104"/>
       <c r="D20" s="22"/>
@@ -4149,7 +4230,7 @@
       <c r="I20" s="14"/>
     </row>
     <row r="21" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="224"/>
+      <c r="A21" s="229"/>
       <c r="B21" s="22"/>
       <c r="D21" s="22"/>
       <c r="E21" s="22"/>
@@ -4159,7 +4240,7 @@
       <c r="I21" s="14"/>
     </row>
     <row r="22" spans="1:9" s="40" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="225"/>
+      <c r="A22" s="230"/>
       <c r="B22" s="54"/>
       <c r="C22" s="54"/>
       <c r="D22" s="54"/>
@@ -4300,7 +4381,7 @@
       <c r="J6" s="14"/>
     </row>
     <row r="7" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="207" t="s">
+      <c r="A7" s="219" t="s">
         <v>40</v>
       </c>
       <c r="B7" s="34"/>
@@ -4313,7 +4394,7 @@
       <c r="I7" s="14"/>
     </row>
     <row r="8" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="207"/>
+      <c r="A8" s="219"/>
       <c r="B8" s="34"/>
       <c r="C8" s="34"/>
       <c r="D8" s="34"/>
@@ -4324,7 +4405,7 @@
       <c r="I8" s="14"/>
     </row>
     <row r="9" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="207"/>
+      <c r="A9" s="219"/>
       <c r="B9" s="34"/>
       <c r="C9" s="34"/>
       <c r="D9" s="34"/>
@@ -4335,7 +4416,7 @@
       <c r="I9" s="14"/>
     </row>
     <row r="10" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="208"/>
+      <c r="A10" s="220"/>
       <c r="B10" s="47"/>
       <c r="C10" s="47"/>
       <c r="D10" s="47"/>
@@ -4346,7 +4427,7 @@
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="209" t="s">
+      <c r="A11" s="212" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="33"/>
@@ -4359,7 +4440,7 @@
       <c r="I11" s="14"/>
     </row>
     <row r="12" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="224"/>
+      <c r="A12" s="229"/>
       <c r="B12" s="34"/>
       <c r="C12" s="34"/>
       <c r="D12" s="34"/>
@@ -4370,7 +4451,7 @@
       <c r="I12" s="14"/>
     </row>
     <row r="13" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="224"/>
+      <c r="A13" s="229"/>
       <c r="B13" s="34"/>
       <c r="C13" s="34"/>
       <c r="D13" s="34"/>
@@ -4381,7 +4462,7 @@
       <c r="I13" s="14"/>
     </row>
     <row r="14" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="226"/>
+      <c r="A14" s="231"/>
       <c r="B14" s="66"/>
       <c r="C14" s="66"/>
       <c r="D14" s="66"/>
@@ -4392,7 +4473,7 @@
       <c r="I14" s="14"/>
     </row>
     <row r="15" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="223" t="s">
+      <c r="A15" s="228" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="12"/>
@@ -4405,7 +4486,7 @@
       <c r="I15" s="14"/>
     </row>
     <row r="16" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="224"/>
+      <c r="A16" s="229"/>
       <c r="B16" s="22"/>
       <c r="C16" s="22"/>
       <c r="D16" s="112"/>
@@ -4416,7 +4497,7 @@
       <c r="I16" s="14"/>
     </row>
     <row r="17" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="224"/>
+      <c r="A17" s="229"/>
       <c r="B17" s="22"/>
       <c r="C17" s="22"/>
       <c r="D17" s="112"/>
@@ -4427,7 +4508,7 @@
       <c r="I17" s="14"/>
     </row>
     <row r="18" spans="1:9" s="40" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="225"/>
+      <c r="A18" s="230"/>
       <c r="B18" s="201"/>
       <c r="C18" s="58"/>
       <c r="D18" s="113"/>
@@ -4577,7 +4658,7 @@
       <c r="J6" s="14"/>
     </row>
     <row r="7" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="207" t="s">
+      <c r="A7" s="219" t="s">
         <v>40</v>
       </c>
       <c r="B7" s="22"/>
@@ -4590,7 +4671,7 @@
       <c r="I7" s="14"/>
     </row>
     <row r="8" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="207"/>
+      <c r="A8" s="219"/>
       <c r="B8" s="22"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
@@ -4601,7 +4682,7 @@
       <c r="I8" s="14"/>
     </row>
     <row r="9" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="207"/>
+      <c r="A9" s="219"/>
       <c r="B9" s="22"/>
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
@@ -4612,7 +4693,7 @@
       <c r="I9" s="14"/>
     </row>
     <row r="10" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="208"/>
+      <c r="A10" s="220"/>
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>
       <c r="D10" s="23"/>
@@ -4623,7 +4704,7 @@
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="228" t="s">
+      <c r="A11" s="234" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="12"/>
@@ -4636,7 +4717,7 @@
       <c r="I11" s="14"/>
     </row>
     <row r="12" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="224"/>
+      <c r="A12" s="229"/>
       <c r="B12" s="22"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
@@ -4647,7 +4728,7 @@
       <c r="I12" s="14"/>
     </row>
     <row r="13" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="224"/>
+      <c r="A13" s="229"/>
       <c r="B13" s="22"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
@@ -4658,7 +4739,7 @@
       <c r="I13" s="14"/>
     </row>
     <row r="14" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="226"/>
+      <c r="A14" s="231"/>
       <c r="B14" s="49"/>
       <c r="C14" s="135"/>
       <c r="D14" s="49"/>
@@ -4669,7 +4750,7 @@
       <c r="I14" s="14"/>
     </row>
     <row r="15" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="223" t="s">
+      <c r="A15" s="228" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="193"/>
@@ -4682,7 +4763,7 @@
       <c r="I15" s="14"/>
     </row>
     <row r="16" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="224"/>
+      <c r="A16" s="229"/>
       <c r="B16" s="22"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
@@ -4693,7 +4774,7 @@
       <c r="I16" s="14"/>
     </row>
     <row r="17" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="224"/>
+      <c r="A17" s="229"/>
       <c r="B17" s="22"/>
       <c r="C17" s="22"/>
       <c r="D17" s="22"/>
@@ -4704,7 +4785,7 @@
       <c r="I17" s="14"/>
     </row>
     <row r="18" spans="1:9" s="40" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="225"/>
+      <c r="A18" s="230"/>
       <c r="B18" s="56"/>
       <c r="C18" s="50"/>
       <c r="D18" s="50"/>
@@ -4843,7 +4924,7 @@
       <c r="J6" s="14"/>
     </row>
     <row r="7" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="207" t="s">
+      <c r="A7" s="219" t="s">
         <v>40</v>
       </c>
       <c r="B7" s="34"/>
@@ -4856,7 +4937,7 @@
       <c r="I7" s="14"/>
     </row>
     <row r="8" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="207"/>
+      <c r="A8" s="219"/>
       <c r="B8" s="34"/>
       <c r="C8" s="34"/>
       <c r="D8" s="34"/>
@@ -4867,7 +4948,7 @@
       <c r="I8" s="14"/>
     </row>
     <row r="9" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="207"/>
+      <c r="A9" s="219"/>
       <c r="B9" s="34"/>
       <c r="C9" s="34"/>
       <c r="D9" s="34"/>
@@ -4878,7 +4959,7 @@
       <c r="I9" s="14"/>
     </row>
     <row r="10" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="208"/>
+      <c r="A10" s="220"/>
       <c r="B10" s="47"/>
       <c r="C10" s="47"/>
       <c r="D10" s="47"/>
@@ -4889,7 +4970,7 @@
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="209" t="s">
+      <c r="A11" s="212" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="33"/>
@@ -4902,7 +4983,7 @@
       <c r="I11" s="14"/>
     </row>
     <row r="12" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="224"/>
+      <c r="A12" s="229"/>
       <c r="B12" s="34"/>
       <c r="C12" s="34"/>
       <c r="D12" s="34"/>
@@ -4913,7 +4994,7 @@
       <c r="I12" s="14"/>
     </row>
     <row r="13" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="224"/>
+      <c r="A13" s="229"/>
       <c r="B13" s="34"/>
       <c r="C13" s="34"/>
       <c r="D13" s="34"/>
@@ -4924,7 +5005,7 @@
       <c r="I13" s="14"/>
     </row>
     <row r="14" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="226"/>
+      <c r="A14" s="231"/>
       <c r="B14" s="60"/>
       <c r="C14" s="134"/>
       <c r="D14" s="60"/>
@@ -4935,7 +5016,7 @@
       <c r="I14" s="14"/>
     </row>
     <row r="15" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="223" t="s">
+      <c r="A15" s="228" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="12"/>
@@ -4948,7 +5029,7 @@
       <c r="I15" s="14"/>
     </row>
     <row r="16" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="224"/>
+      <c r="A16" s="229"/>
       <c r="B16" s="22"/>
       <c r="C16" s="22"/>
       <c r="D16" s="34"/>
@@ -4959,7 +5040,7 @@
       <c r="I16" s="14"/>
     </row>
     <row r="17" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="224"/>
+      <c r="A17" s="229"/>
       <c r="B17" s="22"/>
       <c r="C17" s="22"/>
       <c r="D17" s="34"/>
@@ -4970,7 +5051,7 @@
       <c r="I17" s="14"/>
     </row>
     <row r="18" spans="1:9" s="40" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="225"/>
+      <c r="A18" s="230"/>
       <c r="B18" s="54"/>
       <c r="C18" s="54"/>
       <c r="D18" s="61"/>
@@ -5117,7 +5198,7 @@
       <c r="J6" s="14"/>
     </row>
     <row r="7" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="207" t="s">
+      <c r="A7" s="219" t="s">
         <v>40</v>
       </c>
       <c r="B7" s="22"/>
@@ -5130,7 +5211,7 @@
       <c r="I7" s="14"/>
     </row>
     <row r="8" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="207"/>
+      <c r="A8" s="219"/>
       <c r="B8" s="22"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
@@ -5141,7 +5222,7 @@
       <c r="I8" s="14"/>
     </row>
     <row r="9" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="207"/>
+      <c r="A9" s="219"/>
       <c r="B9" s="22"/>
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
@@ -5152,7 +5233,7 @@
       <c r="I9" s="14"/>
     </row>
     <row r="10" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="208"/>
+      <c r="A10" s="220"/>
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>
       <c r="D10" s="23"/>
@@ -5163,7 +5244,7 @@
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="213" t="s">
+      <c r="A11" s="215" t="s">
         <v>31</v>
       </c>
       <c r="B11" s="22"/>
@@ -5176,7 +5257,7 @@
       <c r="I11" s="14"/>
     </row>
     <row r="12" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="214"/>
+      <c r="A12" s="216"/>
       <c r="B12" s="22"/>
       <c r="C12" s="34"/>
       <c r="D12" s="15"/>
@@ -5187,7 +5268,7 @@
       <c r="I12" s="14"/>
     </row>
     <row r="13" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="214"/>
+      <c r="A13" s="216"/>
       <c r="B13" s="22"/>
       <c r="C13" s="34"/>
       <c r="D13" s="195"/>
@@ -5198,7 +5279,7 @@
       <c r="I13" s="14"/>
     </row>
     <row r="14" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="215"/>
+      <c r="A14" s="217"/>
       <c r="B14" s="102"/>
       <c r="C14" s="200"/>
       <c r="D14" s="196"/>
@@ -5209,7 +5290,7 @@
       <c r="I14" s="14"/>
     </row>
     <row r="15" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="213" t="s">
+      <c r="A15" s="215" t="s">
         <v>32</v>
       </c>
       <c r="B15" s="197"/>
@@ -5222,7 +5303,7 @@
       <c r="I15" s="14"/>
     </row>
     <row r="16" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="214"/>
+      <c r="A16" s="216"/>
       <c r="B16" s="15"/>
       <c r="C16" s="34"/>
       <c r="D16" s="15"/>
@@ -5233,7 +5314,7 @@
       <c r="I16" s="14"/>
     </row>
     <row r="17" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="214"/>
+      <c r="A17" s="216"/>
       <c r="B17" s="15"/>
       <c r="C17" s="34"/>
       <c r="D17" s="98"/>
@@ -5244,7 +5325,7 @@
       <c r="I17" s="14"/>
     </row>
     <row r="18" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="215"/>
+      <c r="A18" s="217"/>
       <c r="B18" s="198"/>
       <c r="C18" s="200"/>
       <c r="D18" s="199"/>
@@ -5255,7 +5336,7 @@
       <c r="I18" s="14"/>
     </row>
     <row r="19" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="210" t="s">
+      <c r="A19" s="213" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="22"/>
@@ -5267,7 +5348,7 @@
       <c r="I19" s="14"/>
     </row>
     <row r="20" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="224"/>
+      <c r="A20" s="229"/>
       <c r="B20" s="22"/>
       <c r="C20" s="34"/>
       <c r="D20" s="22"/>
@@ -5277,7 +5358,7 @@
       <c r="I20" s="14"/>
     </row>
     <row r="21" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="224"/>
+      <c r="A21" s="229"/>
       <c r="B21" s="87"/>
       <c r="C21" s="34"/>
       <c r="D21" s="22"/>
@@ -5287,7 +5368,7 @@
       <c r="I21" s="14"/>
     </row>
     <row r="22" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="226"/>
+      <c r="A22" s="231"/>
       <c r="B22" s="49"/>
       <c r="C22" s="60"/>
       <c r="D22" s="49"/>
@@ -5298,7 +5379,7 @@
       <c r="I22" s="14"/>
     </row>
     <row r="23" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="223" t="s">
+      <c r="A23" s="228" t="s">
         <v>1</v>
       </c>
       <c r="B23" s="94"/>
@@ -5311,7 +5392,7 @@
       <c r="I23" s="14"/>
     </row>
     <row r="24" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="224"/>
+      <c r="A24" s="229"/>
       <c r="B24" s="95"/>
       <c r="C24" s="22"/>
       <c r="D24" s="69"/>
@@ -5322,7 +5403,7 @@
       <c r="I24" s="14"/>
     </row>
     <row r="25" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="224"/>
+      <c r="A25" s="229"/>
       <c r="B25" s="95"/>
       <c r="C25" s="22"/>
       <c r="D25" s="22"/>
@@ -5333,7 +5414,7 @@
       <c r="I25" s="14"/>
     </row>
     <row r="26" spans="1:9" s="40" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="225"/>
+      <c r="A26" s="230"/>
       <c r="B26" s="50"/>
       <c r="C26" s="58"/>
       <c r="D26" s="54"/>
@@ -5465,7 +5546,7 @@
       <c r="J6" s="14"/>
     </row>
     <row r="7" spans="1:10" s="40" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="206" t="s">
+      <c r="A7" s="218" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="12"/>
@@ -5479,7 +5560,7 @@
       <c r="J7" s="14"/>
     </row>
     <row r="8" spans="1:10" s="40" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="207"/>
+      <c r="A8" s="219"/>
       <c r="B8" s="22"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
@@ -5491,7 +5572,7 @@
       <c r="J8" s="14"/>
     </row>
     <row r="9" spans="1:10" s="40" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="207"/>
+      <c r="A9" s="219"/>
       <c r="B9" s="22"/>
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
@@ -5503,7 +5584,7 @@
       <c r="J9" s="14"/>
     </row>
     <row r="10" spans="1:10" s="40" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="208"/>
+      <c r="A10" s="220"/>
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>
       <c r="D10" s="23"/>
@@ -5515,7 +5596,7 @@
       <c r="J10" s="14"/>
     </row>
     <row r="11" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="216" t="s">
+      <c r="A11" s="221" t="s">
         <v>40</v>
       </c>
       <c r="B11" s="12"/>
@@ -5529,7 +5610,7 @@
       <c r="J11" s="14"/>
     </row>
     <row r="12" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="216"/>
+      <c r="A12" s="221"/>
       <c r="B12" s="22"/>
       <c r="C12" s="22"/>
       <c r="D12" s="34"/>
@@ -5541,7 +5622,7 @@
       <c r="J12" s="14"/>
     </row>
     <row r="13" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="216"/>
+      <c r="A13" s="221"/>
       <c r="B13" s="22"/>
       <c r="C13" s="22"/>
       <c r="D13" s="34"/>
@@ -5553,7 +5634,7 @@
       <c r="J13" s="14"/>
     </row>
     <row r="14" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="217"/>
+      <c r="A14" s="222"/>
       <c r="B14" s="53"/>
       <c r="C14" s="23"/>
       <c r="D14" s="66"/>
@@ -5565,7 +5646,7 @@
       <c r="J14" s="14"/>
     </row>
     <row r="15" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="218" t="s">
+      <c r="A15" s="223" t="s">
         <v>35</v>
       </c>
       <c r="B15" s="143"/>
@@ -5579,7 +5660,7 @@
       <c r="J15" s="14"/>
     </row>
     <row r="16" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="219"/>
+      <c r="A16" s="224"/>
       <c r="B16" s="144"/>
       <c r="C16" s="114"/>
       <c r="D16" s="144"/>
@@ -5591,7 +5672,7 @@
       <c r="J16" s="14"/>
     </row>
     <row r="17" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="219"/>
+      <c r="A17" s="224"/>
       <c r="B17" s="144"/>
       <c r="C17" s="88"/>
       <c r="D17" s="144"/>
@@ -5603,7 +5684,7 @@
       <c r="J17" s="14"/>
     </row>
     <row r="18" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="220"/>
+      <c r="A18" s="225"/>
       <c r="B18" s="145"/>
       <c r="C18" s="90"/>
       <c r="D18" s="145"/>
@@ -5615,7 +5696,7 @@
       <c r="J18" s="14"/>
     </row>
     <row r="19" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="219" t="s">
+      <c r="A19" s="224" t="s">
         <v>1</v>
       </c>
       <c r="B19" s="174"/>
@@ -5629,7 +5710,7 @@
       <c r="J19" s="14"/>
     </row>
     <row r="20" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="219"/>
+      <c r="A20" s="224"/>
       <c r="B20" s="22"/>
       <c r="C20" s="29"/>
       <c r="D20" s="150"/>
@@ -5641,7 +5722,7 @@
       <c r="J20" s="14"/>
     </row>
     <row r="21" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="219"/>
+      <c r="A21" s="224"/>
       <c r="B21" s="87"/>
       <c r="C21" s="29"/>
       <c r="D21" s="150"/>
@@ -5653,7 +5734,7 @@
       <c r="J21" s="14"/>
     </row>
     <row r="22" spans="1:10" s="40" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="221"/>
+      <c r="A22" s="226"/>
       <c r="B22" s="54"/>
       <c r="C22" s="54"/>
       <c r="D22" s="187"/>
@@ -5817,7 +5898,7 @@
       <c r="J6" s="14"/>
     </row>
     <row r="7" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="207" t="s">
+      <c r="A7" s="219" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="22"/>
@@ -5830,7 +5911,7 @@
       <c r="I7" s="14"/>
     </row>
     <row r="8" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="207"/>
+      <c r="A8" s="219"/>
       <c r="B8" s="22"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
@@ -5841,7 +5922,7 @@
       <c r="I8" s="14"/>
     </row>
     <row r="9" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="207"/>
+      <c r="A9" s="219"/>
       <c r="B9" s="22"/>
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
@@ -5852,7 +5933,7 @@
       <c r="I9" s="14"/>
     </row>
     <row r="10" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="208"/>
+      <c r="A10" s="220"/>
       <c r="B10" s="53"/>
       <c r="C10" s="23"/>
       <c r="D10" s="53"/>
@@ -5863,7 +5944,7 @@
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="209" t="s">
+      <c r="A11" s="212" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="22"/>
@@ -5876,7 +5957,7 @@
       <c r="I11" s="14"/>
     </row>
     <row r="12" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="224"/>
+      <c r="A12" s="229"/>
       <c r="B12" s="22"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
@@ -5887,7 +5968,7 @@
       <c r="I12" s="14"/>
     </row>
     <row r="13" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="224"/>
+      <c r="A13" s="229"/>
       <c r="B13" s="22"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
@@ -5898,7 +5979,7 @@
       <c r="I13" s="14"/>
     </row>
     <row r="14" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="226"/>
+      <c r="A14" s="231"/>
       <c r="B14" s="49"/>
       <c r="C14" s="53"/>
       <c r="D14" s="23"/>
@@ -5909,7 +5990,7 @@
       <c r="I14" s="14"/>
     </row>
     <row r="15" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="223" t="s">
+      <c r="A15" s="228" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="12"/>
@@ -5922,7 +6003,7 @@
       <c r="I15" s="14"/>
     </row>
     <row r="16" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="224"/>
+      <c r="A16" s="229"/>
       <c r="B16" s="22"/>
       <c r="C16" s="29"/>
       <c r="D16" s="22"/>
@@ -5933,7 +6014,7 @@
       <c r="I16" s="14"/>
     </row>
     <row r="17" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="224"/>
+      <c r="A17" s="229"/>
       <c r="B17" s="22"/>
       <c r="C17" s="29"/>
       <c r="D17" s="22"/>
@@ -5944,7 +6025,7 @@
       <c r="I17" s="14"/>
     </row>
     <row r="18" spans="1:9" s="40" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="225"/>
+      <c r="A18" s="230"/>
       <c r="B18" s="56"/>
       <c r="C18" s="176"/>
       <c r="D18" s="176"/>
@@ -6083,7 +6164,7 @@
       <c r="J6" s="14"/>
     </row>
     <row r="7" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="216" t="s">
+      <c r="A7" s="221" t="s">
         <v>40</v>
       </c>
       <c r="B7" s="22"/>
@@ -6096,7 +6177,7 @@
       <c r="I7" s="14"/>
     </row>
     <row r="8" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="216"/>
+      <c r="A8" s="221"/>
       <c r="B8" s="22"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
@@ -6107,7 +6188,7 @@
       <c r="I8" s="14"/>
     </row>
     <row r="9" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="216"/>
+      <c r="A9" s="221"/>
       <c r="B9" s="22"/>
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
@@ -6118,7 +6199,7 @@
       <c r="I9" s="14"/>
     </row>
     <row r="10" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="217"/>
+      <c r="A10" s="222"/>
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>
       <c r="D10" s="23"/>
@@ -6129,7 +6210,7 @@
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="207" t="s">
+      <c r="A11" s="219" t="s">
         <v>31</v>
       </c>
       <c r="B11" s="22"/>
@@ -6142,7 +6223,7 @@
       <c r="I11" s="14"/>
     </row>
     <row r="12" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="207"/>
+      <c r="A12" s="219"/>
       <c r="B12" s="22"/>
       <c r="C12" s="65"/>
       <c r="D12" s="65"/>
@@ -6153,7 +6234,7 @@
       <c r="I12" s="14"/>
     </row>
     <row r="13" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="207"/>
+      <c r="A13" s="219"/>
       <c r="B13" s="22"/>
       <c r="C13" s="65"/>
       <c r="D13" s="65"/>
@@ -6164,7 +6245,7 @@
       <c r="I13" s="14"/>
     </row>
     <row r="14" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="208"/>
+      <c r="A14" s="220"/>
       <c r="B14" s="49"/>
       <c r="C14" s="60"/>
       <c r="D14" s="60"/>
@@ -6175,7 +6256,7 @@
       <c r="I14" s="14"/>
     </row>
     <row r="15" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="207" t="s">
+      <c r="A15" s="219" t="s">
         <v>32</v>
       </c>
       <c r="B15" s="22"/>
@@ -6188,7 +6269,7 @@
       <c r="I15" s="14"/>
     </row>
     <row r="16" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="207"/>
+      <c r="A16" s="219"/>
       <c r="B16" s="22"/>
       <c r="C16" s="65"/>
       <c r="D16" s="65"/>
@@ -6199,7 +6280,7 @@
       <c r="I16" s="14"/>
     </row>
     <row r="17" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="207"/>
+      <c r="A17" s="219"/>
       <c r="B17" s="22"/>
       <c r="C17" s="65"/>
       <c r="D17" s="65"/>
@@ -6210,7 +6291,7 @@
       <c r="I17" s="14"/>
     </row>
     <row r="18" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="208"/>
+      <c r="A18" s="220"/>
       <c r="B18" s="49"/>
       <c r="C18" s="60"/>
       <c r="D18" s="60"/>
@@ -6221,7 +6302,7 @@
       <c r="I18" s="14"/>
     </row>
     <row r="19" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="209" t="s">
+      <c r="A19" s="212" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="12"/>
@@ -6234,7 +6315,7 @@
       <c r="I19" s="14"/>
     </row>
     <row r="20" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="224"/>
+      <c r="A20" s="229"/>
       <c r="B20" s="22"/>
       <c r="C20" s="65"/>
       <c r="D20" s="65"/>
@@ -6245,7 +6326,7 @@
       <c r="I20" s="14"/>
     </row>
     <row r="21" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="224"/>
+      <c r="A21" s="229"/>
       <c r="B21" s="87"/>
       <c r="C21" s="65"/>
       <c r="D21" s="65"/>
@@ -6256,7 +6337,7 @@
       <c r="I21" s="14"/>
     </row>
     <row r="22" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="226"/>
+      <c r="A22" s="231"/>
       <c r="B22" s="49"/>
       <c r="C22" s="60"/>
       <c r="D22" s="60"/>
@@ -6267,7 +6348,7 @@
       <c r="I22" s="14"/>
     </row>
     <row r="23" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="223" t="s">
+      <c r="A23" s="228" t="s">
         <v>1</v>
       </c>
       <c r="B23" s="12"/>
@@ -6280,7 +6361,7 @@
       <c r="I23" s="14"/>
     </row>
     <row r="24" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="224"/>
+      <c r="A24" s="229"/>
       <c r="B24" s="22"/>
       <c r="C24" s="34"/>
       <c r="D24" s="150"/>
@@ -6291,7 +6372,7 @@
       <c r="I24" s="14"/>
     </row>
     <row r="25" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="224"/>
+      <c r="A25" s="229"/>
       <c r="B25" s="22"/>
       <c r="C25" s="34"/>
       <c r="D25" s="34"/>
@@ -6302,7 +6383,7 @@
       <c r="I25" s="14"/>
     </row>
     <row r="26" spans="1:9" s="40" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="225"/>
+      <c r="A26" s="230"/>
       <c r="B26" s="140"/>
       <c r="C26" s="61"/>
       <c r="D26" s="132"/>
@@ -6440,7 +6521,7 @@
       <c r="J6" s="14"/>
     </row>
     <row r="7" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="207" t="s">
+      <c r="A7" s="219" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="22"/>
@@ -6453,7 +6534,7 @@
       <c r="I7" s="14"/>
     </row>
     <row r="8" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="207"/>
+      <c r="A8" s="219"/>
       <c r="B8" s="22"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
@@ -6464,7 +6545,7 @@
       <c r="I8" s="14"/>
     </row>
     <row r="9" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="207"/>
+      <c r="A9" s="219"/>
       <c r="B9" s="22"/>
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
@@ -6475,7 +6556,7 @@
       <c r="I9" s="14"/>
     </row>
     <row r="10" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="208"/>
+      <c r="A10" s="220"/>
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>
       <c r="D10" s="23"/>
@@ -6486,7 +6567,7 @@
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="209" t="s">
+      <c r="A11" s="212" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="22"/>
@@ -6499,7 +6580,7 @@
       <c r="I11" s="14"/>
     </row>
     <row r="12" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="224"/>
+      <c r="A12" s="229"/>
       <c r="B12" s="22"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
@@ -6510,7 +6591,7 @@
       <c r="I12" s="14"/>
     </row>
     <row r="13" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="224"/>
+      <c r="A13" s="229"/>
       <c r="B13" s="22"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
@@ -6521,7 +6602,7 @@
       <c r="I13" s="14"/>
     </row>
     <row r="14" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="226"/>
+      <c r="A14" s="231"/>
       <c r="B14" s="49"/>
       <c r="C14" s="53"/>
       <c r="D14" s="23"/>
@@ -6532,7 +6613,7 @@
       <c r="I14" s="14"/>
     </row>
     <row r="15" spans="1:10" s="40" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="207" t="s">
+      <c r="A15" s="219" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="22"/>
@@ -6545,7 +6626,7 @@
       <c r="I15" s="14"/>
     </row>
     <row r="16" spans="1:10" s="40" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="207"/>
+      <c r="A16" s="219"/>
       <c r="B16" s="22"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
@@ -6556,7 +6637,7 @@
       <c r="I16" s="14"/>
     </row>
     <row r="17" spans="1:9" s="40" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="207"/>
+      <c r="A17" s="219"/>
       <c r="B17" s="22"/>
       <c r="C17" s="22"/>
       <c r="D17" s="22"/>
@@ -6567,7 +6648,7 @@
       <c r="I17" s="14"/>
     </row>
     <row r="18" spans="1:9" s="40" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="208"/>
+      <c r="A18" s="220"/>
       <c r="B18" s="49"/>
       <c r="C18" s="53"/>
       <c r="D18" s="23"/>
@@ -6578,7 +6659,7 @@
       <c r="I18" s="14"/>
     </row>
     <row r="19" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="223" t="s">
+      <c r="A19" s="228" t="s">
         <v>1</v>
       </c>
       <c r="B19" s="12"/>
@@ -6591,7 +6672,7 @@
       <c r="I19" s="14"/>
     </row>
     <row r="20" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="224"/>
+      <c r="A20" s="229"/>
       <c r="B20" s="22"/>
       <c r="C20" s="22"/>
       <c r="D20" s="22"/>
@@ -6602,7 +6683,7 @@
       <c r="I20" s="14"/>
     </row>
     <row r="21" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="224"/>
+      <c r="A21" s="229"/>
       <c r="B21" s="22"/>
       <c r="C21" s="22"/>
       <c r="D21" s="22"/>
@@ -6613,7 +6694,7 @@
       <c r="I21" s="14"/>
     </row>
     <row r="22" spans="1:9" s="40" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="225"/>
+      <c r="A22" s="230"/>
       <c r="B22" s="56"/>
       <c r="C22" s="50"/>
       <c r="D22" s="56"/>
@@ -6751,7 +6832,7 @@
       <c r="J6" s="14"/>
     </row>
     <row r="7" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="207" t="s">
+      <c r="A7" s="219" t="s">
         <v>40</v>
       </c>
       <c r="B7" s="22"/>
@@ -6764,7 +6845,7 @@
       <c r="I7" s="14"/>
     </row>
     <row r="8" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="207"/>
+      <c r="A8" s="219"/>
       <c r="B8" s="22"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
@@ -6775,7 +6856,7 @@
       <c r="I8" s="14"/>
     </row>
     <row r="9" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="207"/>
+      <c r="A9" s="219"/>
       <c r="B9" s="22"/>
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
@@ -6786,7 +6867,7 @@
       <c r="I9" s="14"/>
     </row>
     <row r="10" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="208"/>
+      <c r="A10" s="220"/>
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>
       <c r="D10" s="23"/>
@@ -6797,7 +6878,7 @@
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="209" t="s">
+      <c r="A11" s="212" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="22"/>
@@ -6810,7 +6891,7 @@
       <c r="I11" s="14"/>
     </row>
     <row r="12" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="224"/>
+      <c r="A12" s="229"/>
       <c r="B12" s="22"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
@@ -6821,7 +6902,7 @@
       <c r="I12" s="14"/>
     </row>
     <row r="13" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="224"/>
+      <c r="A13" s="229"/>
       <c r="B13" s="22"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
@@ -6832,7 +6913,7 @@
       <c r="I13" s="14"/>
     </row>
     <row r="14" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="226"/>
+      <c r="A14" s="231"/>
       <c r="B14" s="49"/>
       <c r="C14" s="53"/>
       <c r="D14" s="23"/>
@@ -6843,7 +6924,7 @@
       <c r="I14" s="14"/>
     </row>
     <row r="15" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="223" t="s">
+      <c r="A15" s="228" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="12"/>
@@ -6856,7 +6937,7 @@
       <c r="I15" s="14"/>
     </row>
     <row r="16" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="224"/>
+      <c r="A16" s="229"/>
       <c r="B16" s="22"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
@@ -6867,7 +6948,7 @@
       <c r="I16" s="14"/>
     </row>
     <row r="17" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="224"/>
+      <c r="A17" s="229"/>
       <c r="B17" s="22"/>
       <c r="C17" s="22"/>
       <c r="D17" s="22"/>
@@ -6878,7 +6959,7 @@
       <c r="I17" s="14"/>
     </row>
     <row r="18" spans="1:9" s="40" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="225"/>
+      <c r="A18" s="230"/>
       <c r="B18" s="92"/>
       <c r="C18" s="166"/>
       <c r="D18" s="56"/>
@@ -7014,7 +7095,7 @@
       <c r="J6" s="14"/>
     </row>
     <row r="7" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="207" t="s">
+      <c r="A7" s="219" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="22"/>
@@ -7027,7 +7108,7 @@
       <c r="I7" s="14"/>
     </row>
     <row r="8" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="207"/>
+      <c r="A8" s="219"/>
       <c r="B8" s="22"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
@@ -7038,7 +7119,7 @@
       <c r="I8" s="14"/>
     </row>
     <row r="9" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="207"/>
+      <c r="A9" s="219"/>
       <c r="B9" s="22"/>
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
@@ -7049,7 +7130,7 @@
       <c r="I9" s="14"/>
     </row>
     <row r="10" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="208"/>
+      <c r="A10" s="220"/>
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>
       <c r="D10" s="23"/>
@@ -7060,7 +7141,7 @@
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="209" t="s">
+      <c r="A11" s="212" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="22"/>
@@ -7073,7 +7154,7 @@
       <c r="I11" s="14"/>
     </row>
     <row r="12" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="224"/>
+      <c r="A12" s="229"/>
       <c r="B12" s="22"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
@@ -7084,7 +7165,7 @@
       <c r="I12" s="14"/>
     </row>
     <row r="13" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="224"/>
+      <c r="A13" s="229"/>
       <c r="B13" s="22"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
@@ -7095,7 +7176,7 @@
       <c r="I13" s="14"/>
     </row>
     <row r="14" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="226"/>
+      <c r="A14" s="231"/>
       <c r="B14" s="49"/>
       <c r="C14" s="53"/>
       <c r="D14" s="23"/>
@@ -7106,7 +7187,7 @@
       <c r="I14" s="14"/>
     </row>
     <row r="15" spans="1:10" s="40" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="207" t="s">
+      <c r="A15" s="219" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="22"/>
@@ -7119,7 +7200,7 @@
       <c r="I15" s="14"/>
     </row>
     <row r="16" spans="1:10" s="40" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="207"/>
+      <c r="A16" s="219"/>
       <c r="B16" s="22"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
@@ -7130,7 +7211,7 @@
       <c r="I16" s="14"/>
     </row>
     <row r="17" spans="1:9" s="40" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="207"/>
+      <c r="A17" s="219"/>
       <c r="B17" s="22"/>
       <c r="C17" s="22"/>
       <c r="D17" s="22"/>
@@ -7141,7 +7222,7 @@
       <c r="I17" s="14"/>
     </row>
     <row r="18" spans="1:9" s="40" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="208"/>
+      <c r="A18" s="220"/>
       <c r="B18" s="49"/>
       <c r="C18" s="53"/>
       <c r="D18" s="23"/>
@@ -7152,7 +7233,7 @@
       <c r="I18" s="14"/>
     </row>
     <row r="19" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="223" t="s">
+      <c r="A19" s="228" t="s">
         <v>1</v>
       </c>
       <c r="B19" s="12"/>
@@ -7165,7 +7246,7 @@
       <c r="I19" s="14"/>
     </row>
     <row r="20" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="224"/>
+      <c r="A20" s="229"/>
       <c r="B20" s="22"/>
       <c r="C20" s="22"/>
       <c r="D20" s="22"/>
@@ -7176,7 +7257,7 @@
       <c r="I20" s="14"/>
     </row>
     <row r="21" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="224"/>
+      <c r="A21" s="229"/>
       <c r="B21" s="22"/>
       <c r="C21" s="22"/>
       <c r="D21" s="22"/>
@@ -7187,7 +7268,7 @@
       <c r="I21" s="14"/>
     </row>
     <row r="22" spans="1:9" s="40" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="225"/>
+      <c r="A22" s="230"/>
       <c r="B22" s="56"/>
       <c r="C22" s="54"/>
       <c r="D22" s="56"/>
@@ -7330,7 +7411,7 @@
       <c r="J6" s="14"/>
     </row>
     <row r="7" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="207" t="s">
+      <c r="A7" s="219" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="22"/>
@@ -7343,7 +7424,7 @@
       <c r="I7" s="14"/>
     </row>
     <row r="8" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="207"/>
+      <c r="A8" s="219"/>
       <c r="B8" s="22"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
@@ -7354,7 +7435,7 @@
       <c r="I8" s="14"/>
     </row>
     <row r="9" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="207"/>
+      <c r="A9" s="219"/>
       <c r="B9" s="22"/>
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
@@ -7365,7 +7446,7 @@
       <c r="I9" s="14"/>
     </row>
     <row r="10" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="208"/>
+      <c r="A10" s="220"/>
       <c r="B10" s="53"/>
       <c r="C10" s="49"/>
       <c r="D10" s="53"/>
@@ -7376,7 +7457,7 @@
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="1:10" s="40" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="213" t="s">
+      <c r="A11" s="215" t="s">
         <v>32</v>
       </c>
       <c r="B11" s="94"/>
@@ -7389,7 +7470,7 @@
       <c r="I11" s="14"/>
     </row>
     <row r="12" spans="1:10" s="40" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="214"/>
+      <c r="A12" s="216"/>
       <c r="B12" s="95"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
@@ -7400,7 +7481,7 @@
       <c r="I12" s="14"/>
     </row>
     <row r="13" spans="1:10" s="40" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="214"/>
+      <c r="A13" s="216"/>
       <c r="B13" s="95"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
@@ -7411,7 +7492,7 @@
       <c r="I13" s="14"/>
     </row>
     <row r="14" spans="1:10" s="40" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="215"/>
+      <c r="A14" s="217"/>
       <c r="B14" s="103"/>
       <c r="C14" s="49"/>
       <c r="D14" s="53"/>
@@ -7422,7 +7503,7 @@
       <c r="I14" s="14"/>
     </row>
     <row r="15" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="210" t="s">
+      <c r="A15" s="213" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="22"/>
@@ -7435,7 +7516,7 @@
       <c r="I15" s="14"/>
     </row>
     <row r="16" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="224"/>
+      <c r="A16" s="229"/>
       <c r="B16" s="22"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
@@ -7446,7 +7527,7 @@
       <c r="I16" s="14"/>
     </row>
     <row r="17" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="224"/>
+      <c r="A17" s="229"/>
       <c r="B17" s="22"/>
       <c r="C17" s="22"/>
       <c r="D17" s="22"/>
@@ -7457,7 +7538,7 @@
       <c r="I17" s="14"/>
     </row>
     <row r="18" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="226"/>
+      <c r="A18" s="231"/>
       <c r="B18" s="49"/>
       <c r="C18" s="53"/>
       <c r="D18" s="23"/>
@@ -7468,7 +7549,7 @@
       <c r="I18" s="14"/>
     </row>
     <row r="19" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="223" t="s">
+      <c r="A19" s="228" t="s">
         <v>1</v>
       </c>
       <c r="B19" s="12"/>
@@ -7481,7 +7562,7 @@
       <c r="I19" s="14"/>
     </row>
     <row r="20" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="224"/>
+      <c r="A20" s="229"/>
       <c r="B20" s="22"/>
       <c r="C20" s="22"/>
       <c r="D20" s="22"/>
@@ -7492,7 +7573,7 @@
       <c r="I20" s="14"/>
     </row>
     <row r="21" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="224"/>
+      <c r="A21" s="229"/>
       <c r="B21" s="22"/>
       <c r="C21" s="22"/>
       <c r="D21" s="22"/>
@@ -7503,7 +7584,7 @@
       <c r="I21" s="14"/>
     </row>
     <row r="22" spans="1:9" s="40" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="225"/>
+      <c r="A22" s="230"/>
       <c r="B22" s="50"/>
       <c r="C22" s="58"/>
       <c r="D22" s="58"/>
@@ -7644,7 +7725,7 @@
       <c r="J6" s="14"/>
     </row>
     <row r="7" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="207" t="s">
+      <c r="A7" s="219" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="34"/>
@@ -7657,7 +7738,7 @@
       <c r="I7" s="14"/>
     </row>
     <row r="8" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="207"/>
+      <c r="A8" s="219"/>
       <c r="B8" s="34"/>
       <c r="C8" s="34"/>
       <c r="D8" s="34"/>
@@ -7668,7 +7749,7 @@
       <c r="I8" s="14"/>
     </row>
     <row r="9" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="207"/>
+      <c r="A9" s="219"/>
       <c r="B9" s="34"/>
       <c r="C9" s="34"/>
       <c r="D9" s="34"/>
@@ -7679,7 +7760,7 @@
       <c r="I9" s="14"/>
     </row>
     <row r="10" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="208"/>
+      <c r="A10" s="220"/>
       <c r="B10" s="66"/>
       <c r="C10" s="47"/>
       <c r="D10" s="66"/>
@@ -7690,7 +7771,7 @@
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="209" t="s">
+      <c r="A11" s="212" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="22"/>
@@ -7703,7 +7784,7 @@
       <c r="I11" s="14"/>
     </row>
     <row r="12" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="224"/>
+      <c r="A12" s="229"/>
       <c r="B12" s="22"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
@@ -7714,7 +7795,7 @@
       <c r="I12" s="14"/>
     </row>
     <row r="13" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="224"/>
+      <c r="A13" s="229"/>
       <c r="B13" s="22"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
@@ -7725,7 +7806,7 @@
       <c r="I13" s="14"/>
     </row>
     <row r="14" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="226"/>
+      <c r="A14" s="231"/>
       <c r="B14" s="49"/>
       <c r="C14" s="49"/>
       <c r="D14" s="49"/>
@@ -7736,7 +7817,7 @@
       <c r="I14" s="14"/>
     </row>
     <row r="15" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="223" t="s">
+      <c r="A15" s="228" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="12"/>
@@ -7749,7 +7830,7 @@
       <c r="I15" s="14"/>
     </row>
     <row r="16" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="224"/>
+      <c r="A16" s="229"/>
       <c r="B16" s="22"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
@@ -7760,7 +7841,7 @@
       <c r="I16" s="14"/>
     </row>
     <row r="17" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="224"/>
+      <c r="A17" s="229"/>
       <c r="B17" s="22"/>
       <c r="C17" s="22"/>
       <c r="D17" s="22"/>
@@ -7771,7 +7852,7 @@
       <c r="I17" s="14"/>
     </row>
     <row r="18" spans="1:9" s="40" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="225"/>
+      <c r="A18" s="230"/>
       <c r="B18" s="54"/>
       <c r="C18" s="54"/>
       <c r="D18" s="107"/>
@@ -7911,7 +7992,7 @@
       <c r="J6" s="14"/>
     </row>
     <row r="7" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="207" t="s">
+      <c r="A7" s="219" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="34"/>
@@ -7924,7 +8005,7 @@
       <c r="I7" s="14"/>
     </row>
     <row r="8" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="207"/>
+      <c r="A8" s="219"/>
       <c r="B8" s="34"/>
       <c r="C8" s="34"/>
       <c r="D8" s="34"/>
@@ -7935,7 +8016,7 @@
       <c r="I8" s="14"/>
     </row>
     <row r="9" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="207"/>
+      <c r="A9" s="219"/>
       <c r="B9" s="34"/>
       <c r="C9" s="34"/>
       <c r="D9" s="34"/>
@@ -7946,7 +8027,7 @@
       <c r="I9" s="14"/>
     </row>
     <row r="10" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="208"/>
+      <c r="A10" s="220"/>
       <c r="B10" s="66"/>
       <c r="C10" s="47"/>
       <c r="D10" s="66"/>
@@ -7957,7 +8038,7 @@
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="209" t="s">
+      <c r="A11" s="212" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="22"/>
@@ -7970,7 +8051,7 @@
       <c r="I11" s="14"/>
     </row>
     <row r="12" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="224"/>
+      <c r="A12" s="229"/>
       <c r="B12" s="22"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
@@ -7981,7 +8062,7 @@
       <c r="I12" s="14"/>
     </row>
     <row r="13" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="224"/>
+      <c r="A13" s="229"/>
       <c r="B13" s="22"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
@@ -7992,7 +8073,7 @@
       <c r="I13" s="14"/>
     </row>
     <row r="14" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="226"/>
+      <c r="A14" s="231"/>
       <c r="B14" s="49"/>
       <c r="C14" s="53"/>
       <c r="D14" s="130"/>
@@ -8003,7 +8084,7 @@
       <c r="I14" s="14"/>
     </row>
     <row r="15" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="223" t="s">
+      <c r="A15" s="228" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="12"/>
@@ -8016,7 +8097,7 @@
       <c r="I15" s="14"/>
     </row>
     <row r="16" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="224"/>
+      <c r="A16" s="229"/>
       <c r="B16" s="22"/>
       <c r="C16" s="29"/>
       <c r="D16" s="22"/>
@@ -8027,7 +8108,7 @@
       <c r="I16" s="14"/>
     </row>
     <row r="17" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="224"/>
+      <c r="A17" s="229"/>
       <c r="B17" s="22"/>
       <c r="C17" s="29"/>
       <c r="D17" s="22"/>
@@ -8038,7 +8119,7 @@
       <c r="I17" s="14"/>
     </row>
     <row r="18" spans="1:9" s="40" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="225"/>
+      <c r="A18" s="230"/>
       <c r="B18" s="54"/>
       <c r="C18" s="166"/>
       <c r="D18" s="54"/>
@@ -8174,7 +8255,7 @@
       <c r="J6" s="14"/>
     </row>
     <row r="7" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="207" t="s">
+      <c r="A7" s="219" t="s">
         <v>40</v>
       </c>
       <c r="B7" s="34"/>
@@ -8186,7 +8267,7 @@
       <c r="H7" s="24"/>
     </row>
     <row r="8" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="207"/>
+      <c r="A8" s="219"/>
       <c r="B8" s="34"/>
       <c r="C8" s="34"/>
       <c r="D8" s="34"/>
@@ -8196,7 +8277,7 @@
       <c r="H8" s="24"/>
     </row>
     <row r="9" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="207"/>
+      <c r="A9" s="219"/>
       <c r="B9" s="34"/>
       <c r="C9" s="34"/>
       <c r="D9" s="34"/>
@@ -8206,7 +8287,7 @@
       <c r="H9" s="24"/>
     </row>
     <row r="10" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="208"/>
+      <c r="A10" s="220"/>
       <c r="B10" s="66"/>
       <c r="C10" s="47"/>
       <c r="D10" s="66"/>
@@ -8216,7 +8297,7 @@
       <c r="H10" s="55"/>
     </row>
     <row r="11" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="209" t="s">
+      <c r="A11" s="212" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="22"/>
@@ -8228,7 +8309,7 @@
       <c r="H11" s="24"/>
     </row>
     <row r="12" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="224"/>
+      <c r="A12" s="229"/>
       <c r="B12" s="22"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
@@ -8238,7 +8319,7 @@
       <c r="H12" s="24"/>
     </row>
     <row r="13" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="224"/>
+      <c r="A13" s="229"/>
       <c r="B13" s="22"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
@@ -8248,7 +8329,7 @@
       <c r="H13" s="24"/>
     </row>
     <row r="14" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="226"/>
+      <c r="A14" s="231"/>
       <c r="B14" s="49"/>
       <c r="C14" s="49"/>
       <c r="D14" s="23"/>
@@ -8258,7 +8339,7 @@
       <c r="H14" s="55"/>
     </row>
     <row r="15" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="223" t="s">
+      <c r="A15" s="228" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="27"/>
@@ -8270,7 +8351,7 @@
       <c r="H15" s="11"/>
     </row>
     <row r="16" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="224"/>
+      <c r="A16" s="229"/>
       <c r="B16" s="22"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
@@ -8280,7 +8361,7 @@
       <c r="H16" s="24"/>
     </row>
     <row r="17" spans="1:8" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="224"/>
+      <c r="A17" s="229"/>
       <c r="B17" s="78"/>
       <c r="C17" s="78"/>
       <c r="D17" s="30"/>
@@ -8290,7 +8371,7 @@
       <c r="H17" s="24"/>
     </row>
     <row r="18" spans="1:8" s="40" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="225"/>
+      <c r="A18" s="230"/>
       <c r="B18" s="50"/>
       <c r="C18" s="50"/>
       <c r="D18" s="50"/>
@@ -8427,7 +8508,7 @@
       <c r="J6" s="14"/>
     </row>
     <row r="7" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="216" t="s">
+      <c r="A7" s="221" t="s">
         <v>40</v>
       </c>
       <c r="B7" s="22"/>
@@ -8439,7 +8520,7 @@
       <c r="H7" s="24"/>
     </row>
     <row r="8" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="216"/>
+      <c r="A8" s="221"/>
       <c r="B8" s="22"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
@@ -8449,7 +8530,7 @@
       <c r="H8" s="24"/>
     </row>
     <row r="9" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="216"/>
+      <c r="A9" s="221"/>
       <c r="B9" s="22"/>
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
@@ -8459,7 +8540,7 @@
       <c r="H9" s="24"/>
     </row>
     <row r="10" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="217"/>
+      <c r="A10" s="222"/>
       <c r="B10" s="53"/>
       <c r="C10" s="23"/>
       <c r="D10" s="53"/>
@@ -8469,7 +8550,7 @@
       <c r="H10" s="55"/>
     </row>
     <row r="11" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="206" t="s">
+      <c r="A11" s="218" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="115"/>
@@ -8481,7 +8562,7 @@
       <c r="H11" s="11"/>
     </row>
     <row r="12" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="207"/>
+      <c r="A12" s="219"/>
       <c r="B12" s="78"/>
       <c r="C12" s="22"/>
       <c r="D12" s="30"/>
@@ -8491,7 +8572,7 @@
       <c r="H12" s="24"/>
     </row>
     <row r="13" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="207"/>
+      <c r="A13" s="219"/>
       <c r="B13" s="30"/>
       <c r="C13" s="22"/>
       <c r="D13" s="30"/>
@@ -8501,7 +8582,7 @@
       <c r="H13" s="24"/>
     </row>
     <row r="14" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="208"/>
+      <c r="A14" s="220"/>
       <c r="B14" s="53"/>
       <c r="C14" s="23"/>
       <c r="D14" s="53"/>
@@ -8511,7 +8592,7 @@
       <c r="H14" s="179"/>
     </row>
     <row r="15" spans="1:10" s="40" customFormat="1" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="210" t="s">
+      <c r="A15" s="213" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="22"/>
@@ -8523,7 +8604,7 @@
       <c r="H15" s="24"/>
     </row>
     <row r="16" spans="1:10" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="224"/>
+      <c r="A16" s="229"/>
       <c r="B16" s="22"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
@@ -8533,7 +8614,7 @@
       <c r="H16" s="24"/>
     </row>
     <row r="17" spans="1:8" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="224"/>
+      <c r="A17" s="229"/>
       <c r="B17" s="22"/>
       <c r="C17" s="22"/>
       <c r="D17" s="22"/>
@@ -8543,7 +8624,7 @@
       <c r="H17" s="24"/>
     </row>
     <row r="18" spans="1:8" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="226"/>
+      <c r="A18" s="231"/>
       <c r="B18" s="31"/>
       <c r="C18" s="49"/>
       <c r="D18" s="23"/>
@@ -8553,7 +8634,7 @@
       <c r="H18" s="63"/>
     </row>
     <row r="19" spans="1:8" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="229" t="s">
+      <c r="A19" s="235" t="s">
         <v>1</v>
       </c>
       <c r="B19" s="12"/>
@@ -8565,7 +8646,7 @@
       <c r="H19" s="11"/>
     </row>
     <row r="20" spans="1:8" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="230"/>
+      <c r="A20" s="236"/>
       <c r="B20" s="69"/>
       <c r="C20" s="22"/>
       <c r="D20" s="22"/>
@@ -8575,7 +8656,7 @@
       <c r="H20" s="24"/>
     </row>
     <row r="21" spans="1:8" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="230"/>
+      <c r="A21" s="236"/>
       <c r="B21" s="69"/>
       <c r="C21" s="22"/>
       <c r="D21" s="22"/>
@@ -8585,7 +8666,7 @@
       <c r="H21" s="24"/>
     </row>
     <row r="22" spans="1:8" s="40" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="231"/>
+      <c r="A22" s="237"/>
       <c r="B22" s="50"/>
       <c r="C22" s="92"/>
       <c r="D22" s="92"/>
@@ -8740,7 +8821,7 @@
       <c r="J6" s="14"/>
     </row>
     <row r="7" spans="1:10" s="40" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="206" t="s">
+      <c r="A7" s="218" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="12"/>
@@ -8754,7 +8835,7 @@
       <c r="J7" s="14"/>
     </row>
     <row r="8" spans="1:10" s="40" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="207"/>
+      <c r="A8" s="219"/>
       <c r="B8" s="22"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
@@ -8766,7 +8847,7 @@
       <c r="J8" s="14"/>
     </row>
     <row r="9" spans="1:10" s="40" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="207"/>
+      <c r="A9" s="219"/>
       <c r="B9" s="22"/>
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
@@ -8778,7 +8859,7 @@
       <c r="J9" s="14"/>
     </row>
     <row r="10" spans="1:10" s="40" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="208"/>
+      <c r="A10" s="220"/>
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>
       <c r="D10" s="23"/>
@@ -8790,7 +8871,7 @@
       <c r="J10" s="14"/>
     </row>
     <row r="11" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="209" t="s">
+      <c r="A11" s="212" t="s">
         <v>31</v>
       </c>
       <c r="B11" s="33"/>
@@ -8804,7 +8885,7 @@
       <c r="J11" s="14"/>
     </row>
     <row r="12" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="210"/>
+      <c r="A12" s="213"/>
       <c r="B12" s="34"/>
       <c r="C12" s="34"/>
       <c r="D12" s="34"/>
@@ -8816,7 +8897,7 @@
       <c r="J12" s="14"/>
     </row>
     <row r="13" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="210"/>
+      <c r="A13" s="213"/>
       <c r="B13" s="34"/>
       <c r="C13" s="34"/>
       <c r="D13" s="34"/>
@@ -8828,7 +8909,7 @@
       <c r="J13" s="14"/>
     </row>
     <row r="14" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="211"/>
+      <c r="A14" s="214"/>
       <c r="B14" s="60"/>
       <c r="C14" s="60"/>
       <c r="D14" s="60"/>
@@ -8840,7 +8921,7 @@
       <c r="J14" s="14"/>
     </row>
     <row r="15" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="222" t="s">
+      <c r="A15" s="227" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="33"/>
@@ -8854,7 +8935,7 @@
       <c r="J15" s="14"/>
     </row>
     <row r="16" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="219"/>
+      <c r="A16" s="224"/>
       <c r="B16" s="34"/>
       <c r="C16" s="34"/>
       <c r="D16" s="34"/>
@@ -8866,7 +8947,7 @@
       <c r="J16" s="14"/>
     </row>
     <row r="17" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="219"/>
+      <c r="A17" s="224"/>
       <c r="B17" s="34"/>
       <c r="C17" s="34"/>
       <c r="D17" s="34"/>
@@ -8878,7 +8959,7 @@
       <c r="J17" s="14"/>
     </row>
     <row r="18" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="220"/>
+      <c r="A18" s="225"/>
       <c r="B18" s="60"/>
       <c r="C18" s="60"/>
       <c r="D18" s="60"/>
@@ -8890,7 +8971,7 @@
       <c r="J18" s="14"/>
     </row>
     <row r="19" spans="1:10" s="40" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="222" t="s">
+      <c r="A19" s="227" t="s">
         <v>35</v>
       </c>
       <c r="B19" s="89"/>
@@ -8904,7 +8985,7 @@
       <c r="J19" s="14"/>
     </row>
     <row r="20" spans="1:10" s="40" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="219"/>
+      <c r="A20" s="224"/>
       <c r="B20" s="88"/>
       <c r="C20" s="22"/>
       <c r="D20" s="30"/>
@@ -8916,7 +8997,7 @@
       <c r="J20" s="14"/>
     </row>
     <row r="21" spans="1:10" s="40" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="219"/>
+      <c r="A21" s="224"/>
       <c r="B21" s="88"/>
       <c r="C21" s="22"/>
       <c r="D21" s="30"/>
@@ -8928,7 +9009,7 @@
       <c r="J21" s="14"/>
     </row>
     <row r="22" spans="1:10" s="40" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="220"/>
+      <c r="A22" s="225"/>
       <c r="B22" s="90"/>
       <c r="C22" s="23"/>
       <c r="D22" s="53"/>
@@ -8940,7 +9021,7 @@
       <c r="J22" s="14"/>
     </row>
     <row r="23" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="219" t="s">
+      <c r="A23" s="224" t="s">
         <v>1</v>
       </c>
       <c r="B23" s="12"/>
@@ -8954,7 +9035,7 @@
       <c r="J23" s="14"/>
     </row>
     <row r="24" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="219"/>
+      <c r="A24" s="224"/>
       <c r="B24" s="22"/>
       <c r="C24" s="22"/>
       <c r="D24" s="22"/>
@@ -8966,7 +9047,7 @@
       <c r="J24" s="14"/>
     </row>
     <row r="25" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="219"/>
+      <c r="A25" s="224"/>
       <c r="B25" s="22"/>
       <c r="C25" s="22"/>
       <c r="D25" s="22"/>
@@ -8978,7 +9059,7 @@
       <c r="J25" s="14"/>
     </row>
     <row r="26" spans="1:10" s="40" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="221"/>
+      <c r="A26" s="226"/>
       <c r="B26" s="58"/>
       <c r="C26" s="54"/>
       <c r="D26" s="107"/>
@@ -9023,6 +9104,246 @@
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8" style="1" customWidth="1"/>
+    <col min="2" max="5" width="14.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" style="51" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="0" style="1" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="17"/>
+      <c r="D2" s="7"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+    </row>
+    <row r="3" spans="1:8" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="18" t="str">
+        <f>[1]Bao!A4</f>
+        <v>Week from 22-02 to 28-02</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="36"/>
+      <c r="B5" s="37">
+        <f>[1]Bao!B6</f>
+        <v>42422</v>
+      </c>
+      <c r="C5" s="37">
+        <f>B5+1</f>
+        <v>42423</v>
+      </c>
+      <c r="D5" s="37">
+        <f t="shared" ref="D5:H5" si="0">C5+1</f>
+        <v>42424</v>
+      </c>
+      <c r="E5" s="37">
+        <f t="shared" si="0"/>
+        <v>42425</v>
+      </c>
+      <c r="F5" s="37">
+        <f t="shared" si="0"/>
+        <v>42426</v>
+      </c>
+      <c r="G5" s="81">
+        <f t="shared" si="0"/>
+        <v>42427</v>
+      </c>
+      <c r="H5" s="82">
+        <f t="shared" si="0"/>
+        <v>42428</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="51" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="218" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="238"/>
+      <c r="C6" s="238"/>
+      <c r="D6" s="238"/>
+      <c r="E6" s="238"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="24"/>
+    </row>
+    <row r="7" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="219"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="24"/>
+    </row>
+    <row r="8" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="219"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="24"/>
+    </row>
+    <row r="9" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="220"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="55"/>
+    </row>
+    <row r="10" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="228" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="24"/>
+    </row>
+    <row r="11" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="229"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="98"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="24"/>
+    </row>
+    <row r="12" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="229"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="24"/>
+    </row>
+    <row r="13" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="231"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="49"/>
+      <c r="H13" s="55"/>
+    </row>
+    <row r="14" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="212" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="12"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="11"/>
+    </row>
+    <row r="15" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="229"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="24"/>
+    </row>
+    <row r="16" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="229"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="239"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="239"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="24"/>
+    </row>
+    <row r="17" spans="1:8" s="51" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="230"/>
+      <c r="B17" s="50"/>
+      <c r="C17" s="64"/>
+      <c r="D17" s="58"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="177"/>
+      <c r="G17" s="54"/>
+      <c r="H17" s="110"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F18" s="51"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="A14:A17"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -9144,7 +9465,7 @@
       <c r="J6" s="14"/>
     </row>
     <row r="7" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="207" t="s">
+      <c r="A7" s="219" t="s">
         <v>40</v>
       </c>
       <c r="B7" s="21"/>
@@ -9158,7 +9479,7 @@
       <c r="J7" s="14"/>
     </row>
     <row r="8" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="207"/>
+      <c r="A8" s="219"/>
       <c r="B8" s="22"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
@@ -9170,7 +9491,7 @@
       <c r="J8" s="14"/>
     </row>
     <row r="9" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="207"/>
+      <c r="A9" s="219"/>
       <c r="B9" s="22"/>
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
@@ -9182,7 +9503,7 @@
       <c r="J9" s="14"/>
     </row>
     <row r="10" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="208"/>
+      <c r="A10" s="220"/>
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>
       <c r="D10" s="23"/>
@@ -9194,7 +9515,7 @@
       <c r="J10" s="14"/>
     </row>
     <row r="11" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="209" t="s">
+      <c r="A11" s="212" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="12"/>
@@ -9208,7 +9529,7 @@
       <c r="J11" s="14"/>
     </row>
     <row r="12" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="224"/>
+      <c r="A12" s="229"/>
       <c r="B12" s="22"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
@@ -9220,7 +9541,7 @@
       <c r="J12" s="14"/>
     </row>
     <row r="13" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="224"/>
+      <c r="A13" s="229"/>
       <c r="B13" s="22"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
@@ -9232,7 +9553,7 @@
       <c r="J13" s="14"/>
     </row>
     <row r="14" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="226"/>
+      <c r="A14" s="231"/>
       <c r="B14" s="49"/>
       <c r="C14" s="49"/>
       <c r="D14" s="53"/>
@@ -9244,7 +9565,7 @@
       <c r="J14" s="14"/>
     </row>
     <row r="15" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="223" t="s">
+      <c r="A15" s="228" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="12"/>
@@ -9258,7 +9579,7 @@
       <c r="J15" s="14"/>
     </row>
     <row r="16" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="224"/>
+      <c r="A16" s="229"/>
       <c r="B16" s="22"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
@@ -9270,7 +9591,7 @@
       <c r="J16" s="14"/>
     </row>
     <row r="17" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="224"/>
+      <c r="A17" s="229"/>
       <c r="B17" s="22"/>
       <c r="C17" s="22"/>
       <c r="D17" s="22"/>
@@ -9282,7 +9603,7 @@
       <c r="J17" s="14"/>
     </row>
     <row r="18" spans="1:10" s="40" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="225"/>
+      <c r="A18" s="230"/>
       <c r="B18" s="58"/>
       <c r="C18" s="54"/>
       <c r="D18" s="54"/>
@@ -9460,7 +9781,7 @@
       <c r="J6" s="14"/>
     </row>
     <row r="7" spans="1:10" s="40" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="206" t="s">
+      <c r="A7" s="218" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="12"/>
@@ -9474,7 +9795,7 @@
       <c r="J7" s="14"/>
     </row>
     <row r="8" spans="1:10" s="40" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="207"/>
+      <c r="A8" s="219"/>
       <c r="B8" s="22"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
@@ -9486,7 +9807,7 @@
       <c r="J8" s="14"/>
     </row>
     <row r="9" spans="1:10" s="40" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="207"/>
+      <c r="A9" s="219"/>
       <c r="B9" s="22"/>
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
@@ -9498,7 +9819,7 @@
       <c r="J9" s="14"/>
     </row>
     <row r="10" spans="1:10" s="40" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="208"/>
+      <c r="A10" s="220"/>
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>
       <c r="D10" s="23"/>
@@ -9510,7 +9831,7 @@
       <c r="J10" s="14"/>
     </row>
     <row r="11" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="216" t="s">
+      <c r="A11" s="221" t="s">
         <v>40</v>
       </c>
       <c r="B11" s="12"/>
@@ -9524,7 +9845,7 @@
       <c r="J11" s="14"/>
     </row>
     <row r="12" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="216"/>
+      <c r="A12" s="221"/>
       <c r="B12" s="22"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
@@ -9536,7 +9857,7 @@
       <c r="J12" s="14"/>
     </row>
     <row r="13" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="216"/>
+      <c r="A13" s="221"/>
       <c r="B13" s="22"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
@@ -9548,7 +9869,7 @@
       <c r="J13" s="14"/>
     </row>
     <row r="14" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="217"/>
+      <c r="A14" s="222"/>
       <c r="B14" s="53"/>
       <c r="C14" s="23"/>
       <c r="D14" s="53"/>
@@ -9560,7 +9881,7 @@
       <c r="J14" s="14"/>
     </row>
     <row r="15" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="218" t="s">
+      <c r="A15" s="223" t="s">
         <v>35</v>
       </c>
       <c r="B15" s="116"/>
@@ -9573,7 +9894,7 @@
       <c r="J15" s="14"/>
     </row>
     <row r="16" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="219"/>
+      <c r="A16" s="224"/>
       <c r="B16" s="114"/>
       <c r="C16" s="114"/>
       <c r="D16" s="114"/>
@@ -9584,7 +9905,7 @@
       <c r="J16" s="14"/>
     </row>
     <row r="17" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="219"/>
+      <c r="A17" s="224"/>
       <c r="B17" s="88"/>
       <c r="C17" s="146"/>
       <c r="D17" s="114"/>
@@ -9595,7 +9916,7 @@
       <c r="J17" s="14"/>
     </row>
     <row r="18" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="220"/>
+      <c r="A18" s="225"/>
       <c r="B18" s="90"/>
       <c r="C18" s="90"/>
       <c r="D18" s="49"/>
@@ -9606,7 +9927,7 @@
       <c r="J18" s="14"/>
     </row>
     <row r="19" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="219" t="s">
+      <c r="A19" s="224" t="s">
         <v>1</v>
       </c>
       <c r="B19" s="108"/>
@@ -9620,7 +9941,7 @@
       <c r="J19" s="14"/>
     </row>
     <row r="20" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="219"/>
+      <c r="A20" s="224"/>
       <c r="B20" s="15"/>
       <c r="C20" s="22"/>
       <c r="D20" s="69"/>
@@ -9632,7 +9953,7 @@
       <c r="J20" s="14"/>
     </row>
     <row r="21" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="219"/>
+      <c r="A21" s="224"/>
       <c r="B21" s="109"/>
       <c r="C21" s="22"/>
       <c r="D21" s="69"/>
@@ -9644,7 +9965,7 @@
       <c r="J21" s="14"/>
     </row>
     <row r="22" spans="1:10" s="40" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="221"/>
+      <c r="A22" s="226"/>
       <c r="B22" s="50"/>
       <c r="C22" s="56"/>
       <c r="D22" s="74"/>
@@ -9793,7 +10114,7 @@
       <c r="J6" s="14"/>
     </row>
     <row r="7" spans="1:10" s="40" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="206" t="s">
+      <c r="A7" s="218" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="12"/>
@@ -9807,7 +10128,7 @@
       <c r="J7" s="14"/>
     </row>
     <row r="8" spans="1:10" s="40" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="207"/>
+      <c r="A8" s="219"/>
       <c r="B8" s="22"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
@@ -9819,7 +10140,7 @@
       <c r="J8" s="14"/>
     </row>
     <row r="9" spans="1:10" s="40" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="207"/>
+      <c r="A9" s="219"/>
       <c r="B9" s="22"/>
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
@@ -9831,7 +10152,7 @@
       <c r="J9" s="14"/>
     </row>
     <row r="10" spans="1:10" s="40" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="208"/>
+      <c r="A10" s="220"/>
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>
       <c r="D10" s="23"/>
@@ -9843,7 +10164,7 @@
       <c r="J10" s="14"/>
     </row>
     <row r="11" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="216" t="s">
+      <c r="A11" s="221" t="s">
         <v>40</v>
       </c>
       <c r="B11" s="12"/>
@@ -9857,7 +10178,7 @@
       <c r="J11" s="14"/>
     </row>
     <row r="12" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="216"/>
+      <c r="A12" s="221"/>
       <c r="B12" s="22"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
@@ -9869,7 +10190,7 @@
       <c r="J12" s="14"/>
     </row>
     <row r="13" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="216"/>
+      <c r="A13" s="221"/>
       <c r="B13" s="22"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
@@ -9881,7 +10202,7 @@
       <c r="J13" s="14"/>
     </row>
     <row r="14" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="217"/>
+      <c r="A14" s="222"/>
       <c r="B14" s="53"/>
       <c r="C14" s="23"/>
       <c r="D14" s="53"/>
@@ -9893,7 +10214,7 @@
       <c r="J14" s="14"/>
     </row>
     <row r="15" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="218" t="s">
+      <c r="A15" s="223" t="s">
         <v>35</v>
       </c>
       <c r="B15" s="116"/>
@@ -9907,7 +10228,7 @@
       <c r="J15" s="14"/>
     </row>
     <row r="16" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="219"/>
+      <c r="A16" s="224"/>
       <c r="B16" s="114"/>
       <c r="C16" s="114"/>
       <c r="D16" s="114"/>
@@ -9919,7 +10240,7 @@
       <c r="J16" s="14"/>
     </row>
     <row r="17" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="219"/>
+      <c r="A17" s="224"/>
       <c r="B17" s="88"/>
       <c r="C17" s="88"/>
       <c r="D17" s="114"/>
@@ -9931,7 +10252,7 @@
       <c r="J17" s="14"/>
     </row>
     <row r="18" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="220"/>
+      <c r="A18" s="225"/>
       <c r="B18" s="90"/>
       <c r="C18" s="90"/>
       <c r="D18" s="90"/>
@@ -9943,7 +10264,7 @@
       <c r="J18" s="14"/>
     </row>
     <row r="19" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="219" t="s">
+      <c r="A19" s="224" t="s">
         <v>1</v>
       </c>
       <c r="B19" s="12"/>
@@ -9957,7 +10278,7 @@
       <c r="J19" s="14"/>
     </row>
     <row r="20" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="219"/>
+      <c r="A20" s="224"/>
       <c r="B20" s="22"/>
       <c r="C20" s="29"/>
       <c r="D20" s="22"/>
@@ -9969,7 +10290,7 @@
       <c r="J20" s="14"/>
     </row>
     <row r="21" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="219"/>
+      <c r="A21" s="224"/>
       <c r="B21" s="22"/>
       <c r="C21" s="29"/>
       <c r="D21" s="22"/>
@@ -9981,7 +10302,7 @@
       <c r="J21" s="14"/>
     </row>
     <row r="22" spans="1:10" s="40" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="221"/>
+      <c r="A22" s="226"/>
       <c r="B22" s="50"/>
       <c r="C22" s="50"/>
       <c r="D22" s="50"/>
@@ -10135,7 +10456,7 @@
       <c r="J6" s="14"/>
     </row>
     <row r="7" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="216" t="s">
+      <c r="A7" s="221" t="s">
         <v>40</v>
       </c>
       <c r="B7" s="22"/>
@@ -10148,7 +10469,7 @@
       <c r="I7" s="14"/>
     </row>
     <row r="8" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="216"/>
+      <c r="A8" s="221"/>
       <c r="B8" s="22"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
@@ -10159,7 +10480,7 @@
       <c r="I8" s="14"/>
     </row>
     <row r="9" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="216"/>
+      <c r="A9" s="221"/>
       <c r="B9" s="22"/>
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
@@ -10170,7 +10491,7 @@
       <c r="I9" s="14"/>
     </row>
     <row r="10" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="217"/>
+      <c r="A10" s="222"/>
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>
       <c r="D10" s="53"/>
@@ -10181,7 +10502,7 @@
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="209" t="s">
+      <c r="A11" s="212" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="12"/>
@@ -10194,7 +10515,7 @@
       <c r="I11" s="14"/>
     </row>
     <row r="12" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="224"/>
+      <c r="A12" s="229"/>
       <c r="B12" s="22"/>
       <c r="C12" s="22"/>
       <c r="D12" s="34"/>
@@ -10205,7 +10526,7 @@
       <c r="I12" s="14"/>
     </row>
     <row r="13" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="224"/>
+      <c r="A13" s="229"/>
       <c r="B13" s="22"/>
       <c r="C13" s="22"/>
       <c r="D13" s="34"/>
@@ -10216,7 +10537,7 @@
       <c r="I13" s="14"/>
     </row>
     <row r="14" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="226"/>
+      <c r="A14" s="231"/>
       <c r="B14" s="53"/>
       <c r="C14" s="53"/>
       <c r="D14" s="66"/>
@@ -10227,7 +10548,7 @@
       <c r="I14" s="14"/>
     </row>
     <row r="15" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="223" t="s">
+      <c r="A15" s="228" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="12"/>
@@ -10240,7 +10561,7 @@
       <c r="I15" s="14"/>
     </row>
     <row r="16" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="224"/>
+      <c r="A16" s="229"/>
       <c r="B16" s="22"/>
       <c r="C16" s="22"/>
       <c r="D16" s="34"/>
@@ -10251,7 +10572,7 @@
       <c r="I16" s="14"/>
     </row>
     <row r="17" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="224"/>
+      <c r="A17" s="229"/>
       <c r="B17" s="22"/>
       <c r="C17" s="22"/>
       <c r="D17" s="34"/>
@@ -10262,7 +10583,7 @@
       <c r="I17" s="14"/>
     </row>
     <row r="18" spans="1:9" s="40" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="225"/>
+      <c r="A18" s="230"/>
       <c r="B18" s="56"/>
       <c r="C18" s="50"/>
       <c r="D18" s="61"/>
@@ -10488,7 +10809,7 @@
       <c r="J6" s="14"/>
     </row>
     <row r="7" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="207" t="s">
+      <c r="A7" s="219" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="22"/>
@@ -10501,7 +10822,7 @@
       <c r="I7" s="14"/>
     </row>
     <row r="8" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="207"/>
+      <c r="A8" s="219"/>
       <c r="B8" s="22"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
@@ -10511,7 +10832,7 @@
       <c r="I8" s="14"/>
     </row>
     <row r="9" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="207"/>
+      <c r="A9" s="219"/>
       <c r="B9" s="22"/>
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
@@ -10522,7 +10843,7 @@
       <c r="I9" s="14"/>
     </row>
     <row r="10" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="208"/>
+      <c r="A10" s="220"/>
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>
       <c r="D10" s="23"/>
@@ -10533,7 +10854,7 @@
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="209" t="s">
+      <c r="A11" s="212" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="12"/>
@@ -10546,7 +10867,7 @@
       <c r="I11" s="14"/>
     </row>
     <row r="12" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="210"/>
+      <c r="A12" s="213"/>
       <c r="B12" s="22"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
@@ -10557,7 +10878,7 @@
       <c r="I12" s="14"/>
     </row>
     <row r="13" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="210"/>
+      <c r="A13" s="213"/>
       <c r="B13" s="22"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
@@ -10568,7 +10889,7 @@
       <c r="I13" s="14"/>
     </row>
     <row r="14" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="211"/>
+      <c r="A14" s="214"/>
       <c r="B14" s="49"/>
       <c r="C14" s="49"/>
       <c r="D14" s="49"/>
@@ -10579,7 +10900,7 @@
       <c r="I14" s="14"/>
     </row>
     <row r="15" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="209" t="s">
+      <c r="A15" s="212" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="12"/>
@@ -10592,7 +10913,7 @@
       <c r="I15" s="14"/>
     </row>
     <row r="16" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="210"/>
+      <c r="A16" s="213"/>
       <c r="B16" s="22"/>
       <c r="C16" s="34"/>
       <c r="D16" s="22"/>
@@ -10603,7 +10924,7 @@
       <c r="I16" s="14"/>
     </row>
     <row r="17" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="210"/>
+      <c r="A17" s="213"/>
       <c r="B17" s="22"/>
       <c r="C17" s="34"/>
       <c r="D17" s="22"/>
@@ -10614,7 +10935,7 @@
       <c r="I17" s="14"/>
     </row>
     <row r="18" spans="1:9" s="40" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="212"/>
+      <c r="A18" s="232"/>
       <c r="B18" s="54"/>
       <c r="C18" s="122"/>
       <c r="D18" s="54"/>
@@ -10749,7 +11070,7 @@
       <c r="J6" s="14"/>
     </row>
     <row r="7" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="207" t="s">
+      <c r="A7" s="219" t="s">
         <v>40</v>
       </c>
       <c r="B7" s="22"/>
@@ -10762,7 +11083,7 @@
       <c r="I7" s="14"/>
     </row>
     <row r="8" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="207"/>
+      <c r="A8" s="219"/>
       <c r="B8" s="22"/>
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
@@ -10773,7 +11094,7 @@
       <c r="I8" s="14"/>
     </row>
     <row r="9" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="207"/>
+      <c r="A9" s="219"/>
       <c r="B9" s="22"/>
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
@@ -10784,7 +11105,7 @@
       <c r="I9" s="14"/>
     </row>
     <row r="10" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="208"/>
+      <c r="A10" s="220"/>
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>
       <c r="D10" s="23"/>
@@ -10795,7 +11116,7 @@
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="209" t="s">
+      <c r="A11" s="212" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="22"/>
@@ -10808,7 +11129,7 @@
       <c r="I11" s="14"/>
     </row>
     <row r="12" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="210"/>
+      <c r="A12" s="213"/>
       <c r="B12" s="22"/>
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
@@ -10819,7 +11140,7 @@
       <c r="I12" s="14"/>
     </row>
     <row r="13" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="210"/>
+      <c r="A13" s="213"/>
       <c r="B13" s="22"/>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
@@ -10830,7 +11151,7 @@
       <c r="I13" s="14"/>
     </row>
     <row r="14" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="211"/>
+      <c r="A14" s="214"/>
       <c r="B14" s="49"/>
       <c r="C14" s="53"/>
       <c r="D14" s="23"/>
@@ -10841,7 +11162,7 @@
       <c r="I14" s="14"/>
     </row>
     <row r="15" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="209" t="s">
+      <c r="A15" s="212" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="94"/>
@@ -10854,7 +11175,7 @@
       <c r="I15" s="14"/>
     </row>
     <row r="16" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="210"/>
+      <c r="A16" s="213"/>
       <c r="B16" s="95"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
@@ -10865,7 +11186,7 @@
       <c r="I16" s="14"/>
     </row>
     <row r="17" spans="1:9" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="210"/>
+      <c r="A17" s="213"/>
       <c r="B17" s="95"/>
       <c r="C17" s="22"/>
       <c r="D17" s="22"/>
@@ -10876,7 +11197,7 @@
       <c r="I17" s="14"/>
     </row>
     <row r="18" spans="1:9" s="40" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="212"/>
+      <c r="A18" s="232"/>
       <c r="B18" s="201"/>
       <c r="C18" s="201"/>
       <c r="D18" s="54"/>

</xml_diff>